<commit_message>
Fix Excel Distancias Merida/LaPaz
</commit_message>
<xml_diff>
--- a/Rutas_Cemix_Origen_TodosDestinos.xlsx
+++ b/Rutas_Cemix_Origen_TodosDestinos.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Cemix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\PycharmProjects\DS-de-Cimex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1433BAA-79E4-4D26-8B4A-EE4E419527DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EEF88A-CC96-4B82-81DE-021EC05040DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="10920" xr2:uid="{ABC5CFBD-A642-4244-A295-C882748C920D}"/>
   </bookViews>
@@ -900,15 +900,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2AB4770-D27B-4A3E-A38A-755CF371868C}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J2619"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2598" workbookViewId="0">
-      <selection activeCell="E2613" sqref="E2613"/>
+    <sheetView tabSelected="1" topLeftCell="A1083" workbookViewId="0">
+      <selection activeCell="C1085" sqref="C1085"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
@@ -5615,7 +5616,7 @@
       <c r="B325" t="s">
         <v>17</v>
       </c>
-      <c r="C325" s="4">
+      <c r="C325">
         <v>692.9470455548543</v>
       </c>
       <c r="E325" s="3"/>
@@ -5627,7 +5628,7 @@
       <c r="B326" t="s">
         <v>18</v>
       </c>
-      <c r="C326" s="4">
+      <c r="C326">
         <v>885.20669497148197</v>
       </c>
       <c r="E326" s="3"/>
@@ -5639,7 +5640,7 @@
       <c r="B327" t="s">
         <v>19</v>
       </c>
-      <c r="C327" s="4">
+      <c r="C327">
         <v>1150.0703779607113</v>
       </c>
       <c r="E327" s="3"/>
@@ -5651,7 +5652,7 @@
       <c r="B328" t="s">
         <v>20</v>
       </c>
-      <c r="C328" s="4">
+      <c r="C328">
         <v>1006.7505965275366</v>
       </c>
       <c r="E328" s="3"/>
@@ -5663,7 +5664,7 @@
       <c r="B329" t="s">
         <v>118</v>
       </c>
-      <c r="C329" s="4">
+      <c r="C329">
         <v>1158.2389151408797</v>
       </c>
       <c r="E329" s="3"/>
@@ -5675,7 +5676,7 @@
       <c r="B330" t="s">
         <v>3</v>
       </c>
-      <c r="C330" s="4">
+      <c r="C330">
         <v>1225.4236262360214</v>
       </c>
       <c r="E330" s="3"/>
@@ -5687,7 +5688,7 @@
       <c r="B331" t="s">
         <v>119</v>
       </c>
-      <c r="C331" s="4">
+      <c r="C331">
         <v>369.21242101660999</v>
       </c>
       <c r="E331" s="3"/>
@@ -5699,7 +5700,7 @@
       <c r="B332" t="s">
         <v>21</v>
       </c>
-      <c r="C332" s="4">
+      <c r="C332">
         <v>705.20789561034485</v>
       </c>
       <c r="E332" s="3"/>
@@ -5711,7 +5712,7 @@
       <c r="B333" t="s">
         <v>22</v>
       </c>
-      <c r="C333" s="4">
+      <c r="C333">
         <v>213.35371817323306</v>
       </c>
       <c r="E333" s="3"/>
@@ -5723,7 +5724,7 @@
       <c r="B334" t="s">
         <v>120</v>
       </c>
-      <c r="C334" s="4">
+      <c r="C334">
         <v>452.37160932622476</v>
       </c>
       <c r="E334" s="3"/>
@@ -5735,7 +5736,7 @@
       <c r="B335" t="s">
         <v>6</v>
       </c>
-      <c r="C335" s="4">
+      <c r="C335">
         <v>460.34294920257878</v>
       </c>
       <c r="E335" s="3"/>
@@ -5747,7 +5748,7 @@
       <c r="B336" t="s">
         <v>23</v>
       </c>
-      <c r="C336" s="4">
+      <c r="C336">
         <v>172.69108762435241</v>
       </c>
       <c r="E336" s="3"/>
@@ -5759,7 +5760,7 @@
       <c r="B337" t="s">
         <v>121</v>
       </c>
-      <c r="C337" s="4">
+      <c r="C337">
         <v>1506.5709976835965</v>
       </c>
       <c r="E337" s="3"/>
@@ -5771,7 +5772,7 @@
       <c r="B338" t="s">
         <v>24</v>
       </c>
-      <c r="C338" s="4">
+      <c r="C338">
         <v>86.395448454908816</v>
       </c>
       <c r="E338" s="3"/>
@@ -5783,7 +5784,7 @@
       <c r="B339" t="s">
         <v>122</v>
       </c>
-      <c r="C339" s="4">
+      <c r="C339">
         <v>1266.109450934375</v>
       </c>
       <c r="E339" s="3"/>
@@ -5795,7 +5796,7 @@
       <c r="B340" t="s">
         <v>26</v>
       </c>
-      <c r="C340" s="4">
+      <c r="C340">
         <v>1294.8975884469862</v>
       </c>
       <c r="E340" s="3"/>
@@ -5807,7 +5808,7 @@
       <c r="B341" t="s">
         <v>27</v>
       </c>
-      <c r="C341" s="4">
+      <c r="C341">
         <v>770.20872652214587</v>
       </c>
       <c r="E341" s="3"/>
@@ -5819,7 +5820,7 @@
       <c r="B342" t="s">
         <v>29</v>
       </c>
-      <c r="C342" s="4">
+      <c r="C342">
         <v>1227.0952044566877</v>
       </c>
       <c r="E342" s="3"/>
@@ -5831,7 +5832,7 @@
       <c r="B343" t="s">
         <v>123</v>
       </c>
-      <c r="C343" s="4">
+      <c r="C343">
         <v>702.20388059687593</v>
       </c>
       <c r="E343" s="3"/>
@@ -5843,7 +5844,7 @@
       <c r="B344" t="s">
         <v>124</v>
       </c>
-      <c r="C344" s="4">
+      <c r="C344">
         <v>1040.0978426687807</v>
       </c>
       <c r="E344" s="3"/>
@@ -5855,7 +5856,7 @@
       <c r="B345" t="s">
         <v>30</v>
       </c>
-      <c r="C345" s="4">
+      <c r="C345">
         <v>107.26751991582893</v>
       </c>
       <c r="E345" s="3"/>
@@ -5867,7 +5868,7 @@
       <c r="B346" t="s">
         <v>31</v>
       </c>
-      <c r="C346" s="4">
+      <c r="C346">
         <v>743.04909255491941</v>
       </c>
       <c r="E346" s="3"/>
@@ -5879,7 +5880,7 @@
       <c r="B347" t="s">
         <v>32</v>
       </c>
-      <c r="C347" s="4">
+      <c r="C347">
         <v>635.3751151481182</v>
       </c>
       <c r="E347" s="3"/>
@@ -5891,7 +5892,7 @@
       <c r="B348" t="s">
         <v>33</v>
       </c>
-      <c r="C348" s="4">
+      <c r="C348">
         <v>808.96499115291476</v>
       </c>
       <c r="E348" s="3"/>
@@ -5903,7 +5904,7 @@
       <c r="B349" t="s">
         <v>34</v>
       </c>
-      <c r="C349" s="4">
+      <c r="C349">
         <v>1608.5927757566528</v>
       </c>
       <c r="E349" s="3"/>
@@ -5915,7 +5916,7 @@
       <c r="B350" t="s">
         <v>35</v>
       </c>
-      <c r="C350" s="4">
+      <c r="C350">
         <v>862.46631303510583</v>
       </c>
       <c r="E350" s="3"/>
@@ -5927,7 +5928,7 @@
       <c r="B351" t="s">
         <v>36</v>
       </c>
-      <c r="C351" s="4">
+      <c r="C351">
         <v>699.36106474473979</v>
       </c>
       <c r="E351" s="3"/>
@@ -5939,7 +5940,7 @@
       <c r="B352" t="s">
         <v>37</v>
       </c>
-      <c r="C352" s="4">
+      <c r="C352">
         <v>427.47573644794733</v>
       </c>
       <c r="E352" s="3"/>
@@ -5951,7 +5952,7 @@
       <c r="B353" t="s">
         <v>38</v>
       </c>
-      <c r="C353" s="4">
+      <c r="C353">
         <v>1542.6340822584768</v>
       </c>
       <c r="E353" s="3"/>
@@ -5963,7 +5964,7 @@
       <c r="B354" t="s">
         <v>39</v>
       </c>
-      <c r="C354" s="4">
+      <c r="C354">
         <v>515.15080926441919</v>
       </c>
       <c r="E354" s="3"/>
@@ -5975,7 +5976,7 @@
       <c r="B355" t="s">
         <v>40</v>
       </c>
-      <c r="C355" s="4">
+      <c r="C355">
         <v>1038.7557683583104</v>
       </c>
       <c r="E355" s="3"/>
@@ -5987,7 +5988,7 @@
       <c r="B356" t="s">
         <v>41</v>
       </c>
-      <c r="C356" s="4">
+      <c r="C356">
         <v>217.8275722175413</v>
       </c>
       <c r="E356" s="3"/>
@@ -5999,7 +6000,7 @@
       <c r="B357" t="s">
         <v>9</v>
       </c>
-      <c r="C357" s="4">
+      <c r="C357">
         <v>2187.5879259966969</v>
       </c>
       <c r="E357" s="3"/>
@@ -6011,7 +6012,7 @@
       <c r="B358" t="s">
         <v>42</v>
       </c>
-      <c r="C358" s="4">
+      <c r="C358">
         <v>325.54304798275223</v>
       </c>
       <c r="E358" s="3"/>
@@ -6023,7 +6024,7 @@
       <c r="B359" t="s">
         <v>125</v>
       </c>
-      <c r="C359" s="4">
+      <c r="C359">
         <v>736.49963941416763</v>
       </c>
       <c r="E359" s="3"/>
@@ -6035,7 +6036,7 @@
       <c r="B360" t="s">
         <v>43</v>
       </c>
-      <c r="C360" s="4">
+      <c r="C360">
         <v>1279.1713302442058</v>
       </c>
       <c r="E360" s="3"/>
@@ -6047,7 +6048,7 @@
       <c r="B361" t="s">
         <v>44</v>
       </c>
-      <c r="C361" s="4">
+      <c r="C361">
         <v>1160.6660639867453</v>
       </c>
       <c r="E361" s="3"/>
@@ -6059,7 +6060,7 @@
       <c r="B362" t="s">
         <v>45</v>
       </c>
-      <c r="C362" s="4">
+      <c r="C362">
         <v>763.26411880549449</v>
       </c>
       <c r="E362" s="3"/>
@@ -6071,7 +6072,7 @@
       <c r="B363" t="s">
         <v>126</v>
       </c>
-      <c r="C363" s="4">
+      <c r="C363">
         <v>1166.8294843197446</v>
       </c>
       <c r="E363" s="3"/>
@@ -6083,7 +6084,7 @@
       <c r="B364" t="s">
         <v>127</v>
       </c>
-      <c r="C364" s="4">
+      <c r="C364">
         <v>649.87360610594271</v>
       </c>
       <c r="E364" s="3"/>
@@ -6095,7 +6096,7 @@
       <c r="B365" t="s">
         <v>46</v>
       </c>
-      <c r="C365" s="4">
+      <c r="C365">
         <v>353.66745415776444</v>
       </c>
       <c r="E365" s="3"/>
@@ -6107,7 +6108,7 @@
       <c r="B366" t="s">
         <v>47</v>
       </c>
-      <c r="C366" s="4">
+      <c r="C366">
         <v>478.84616753133486</v>
       </c>
       <c r="E366" s="3"/>
@@ -6119,7 +6120,7 @@
       <c r="B367" t="s">
         <v>48</v>
       </c>
-      <c r="C367" s="4">
+      <c r="C367">
         <v>354.11463090449018</v>
       </c>
       <c r="E367" s="3"/>
@@ -6131,7 +6132,7 @@
       <c r="B368" t="s">
         <v>128</v>
       </c>
-      <c r="C368" s="4">
+      <c r="C368">
         <v>1067.6214618039678</v>
       </c>
       <c r="E368" s="3"/>
@@ -6143,7 +6144,7 @@
       <c r="B369" t="s">
         <v>49</v>
       </c>
-      <c r="C369" s="4">
+      <c r="C369">
         <v>204.38965687303215</v>
       </c>
       <c r="E369" s="3"/>
@@ -6155,7 +6156,7 @@
       <c r="B370" t="s">
         <v>50</v>
       </c>
-      <c r="C370" s="4">
+      <c r="C370">
         <v>725.27523106611193</v>
       </c>
       <c r="E370" s="3"/>
@@ -6167,7 +6168,7 @@
       <c r="B371" t="s">
         <v>51</v>
       </c>
-      <c r="C371" s="4">
+      <c r="C371">
         <v>2225.5124931822029</v>
       </c>
       <c r="E371" s="3"/>
@@ -6179,7 +6180,7 @@
       <c r="B372" t="s">
         <v>52</v>
       </c>
-      <c r="C372" s="4">
+      <c r="C372">
         <v>252.03344399097637</v>
       </c>
       <c r="E372" s="3"/>
@@ -6191,7 +6192,7 @@
       <c r="B373" t="s">
         <v>16</v>
       </c>
-      <c r="C373" s="4">
+      <c r="C373">
         <v>672.01230591111732</v>
       </c>
       <c r="E373" s="3"/>
@@ -6203,7 +6204,7 @@
       <c r="B374" t="s">
         <v>53</v>
       </c>
-      <c r="C374" s="4">
+      <c r="C374">
         <v>1143.458196002618</v>
       </c>
       <c r="E374" s="3"/>
@@ -6215,7 +6216,7 @@
       <c r="B375" t="s">
         <v>54</v>
       </c>
-      <c r="C375" s="4">
+      <c r="C375">
         <v>864.24496601025101</v>
       </c>
       <c r="E375" s="3"/>
@@ -6227,7 +6228,7 @@
       <c r="B376" t="s">
         <v>55</v>
       </c>
-      <c r="C376" s="4">
+      <c r="C376">
         <v>802.90840514853573</v>
       </c>
       <c r="E376" s="3"/>
@@ -6239,7 +6240,7 @@
       <c r="B377" t="s">
         <v>56</v>
       </c>
-      <c r="C377" s="4">
+      <c r="C377">
         <v>108.7769127849463</v>
       </c>
       <c r="E377" s="3"/>
@@ -6251,7 +6252,7 @@
       <c r="B378" t="s">
         <v>57</v>
       </c>
-      <c r="C378" s="4">
+      <c r="C378">
         <v>2293.6133069396337</v>
       </c>
       <c r="E378" s="3"/>
@@ -6263,7 +6264,7 @@
       <c r="B379" t="s">
         <v>58</v>
       </c>
-      <c r="C379" s="4">
+      <c r="C379">
         <v>190.88688400370984</v>
       </c>
       <c r="E379" s="3"/>
@@ -6275,7 +6276,7 @@
       <c r="B380" t="s">
         <v>59</v>
       </c>
-      <c r="C380" s="4">
+      <c r="C380">
         <v>296.28092413463992</v>
       </c>
       <c r="E380" s="3"/>
@@ -6287,7 +6288,7 @@
       <c r="B381" t="s">
         <v>15</v>
       </c>
-      <c r="C381" s="4">
+      <c r="C381">
         <v>315.81510437756668</v>
       </c>
       <c r="E381" s="3"/>
@@ -6299,7 +6300,7 @@
       <c r="B382" t="s">
         <v>129</v>
       </c>
-      <c r="C382" s="4">
+      <c r="C382">
         <v>1308.0199071341444</v>
       </c>
       <c r="E382" s="3"/>
@@ -6311,7 +6312,7 @@
       <c r="B383" t="s">
         <v>60</v>
       </c>
-      <c r="C383" s="4">
+      <c r="C383">
         <v>513.49468811876636</v>
       </c>
       <c r="E383" s="3"/>
@@ -6323,7 +6324,7 @@
       <c r="B384" t="s">
         <v>130</v>
       </c>
-      <c r="C384" s="4">
+      <c r="C384">
         <v>895.26021108585223</v>
       </c>
       <c r="E384" s="3"/>
@@ -6335,7 +6336,7 @@
       <c r="B385" t="s">
         <v>62</v>
       </c>
-      <c r="C385" s="4">
+      <c r="C385">
         <v>304.2477274964437</v>
       </c>
       <c r="E385" s="3"/>
@@ -6347,7 +6348,7 @@
       <c r="B386" t="s">
         <v>7</v>
       </c>
-      <c r="C386" s="4">
+      <c r="C386">
         <v>1266.870682206918</v>
       </c>
       <c r="E386" s="3"/>
@@ -6359,7 +6360,7 @@
       <c r="B387" t="s">
         <v>131</v>
       </c>
-      <c r="C387" s="4">
+      <c r="C387">
         <v>814.88889625327749</v>
       </c>
       <c r="E387" s="3"/>
@@ -6371,7 +6372,7 @@
       <c r="B388" t="s">
         <v>63</v>
       </c>
-      <c r="C388" s="4">
+      <c r="C388">
         <v>740.14504115985392</v>
       </c>
       <c r="E388" s="3"/>
@@ -6383,7 +6384,7 @@
       <c r="B389" t="s">
         <v>64</v>
       </c>
-      <c r="C389" s="4">
+      <c r="C389">
         <v>1421.9063243641403</v>
       </c>
       <c r="E389" s="3"/>
@@ -6395,7 +6396,7 @@
       <c r="B390" t="s">
         <v>65</v>
       </c>
-      <c r="C390" s="4">
+      <c r="C390">
         <v>260.46791085894472</v>
       </c>
       <c r="E390" s="3"/>
@@ -6407,7 +6408,7 @@
       <c r="B391" t="s">
         <v>12</v>
       </c>
-      <c r="C391" s="4">
+      <c r="C391">
         <v>338.26421903856141</v>
       </c>
       <c r="E391" s="3"/>
@@ -6419,7 +6420,7 @@
       <c r="B392" t="s">
         <v>66</v>
       </c>
-      <c r="C392" s="4">
+      <c r="C392">
         <v>642.819495306401</v>
       </c>
       <c r="E392" s="3"/>
@@ -6431,7 +6432,7 @@
       <c r="B393" t="s">
         <v>67</v>
       </c>
-      <c r="C393" s="4">
+      <c r="C393">
         <v>733.15248349731371</v>
       </c>
       <c r="E393" s="3"/>
@@ -6443,7 +6444,7 @@
       <c r="B394" t="s">
         <v>132</v>
       </c>
-      <c r="C394" s="4">
+      <c r="C394">
         <v>1960.2621517309826</v>
       </c>
       <c r="E394" s="3"/>
@@ -6455,7 +6456,7 @@
       <c r="B395" t="s">
         <v>68</v>
       </c>
-      <c r="C395" s="4">
+      <c r="C395">
         <v>905.04809029955641</v>
       </c>
       <c r="E395" s="3"/>
@@ -6467,7 +6468,7 @@
       <c r="B396" t="s">
         <v>69</v>
       </c>
-      <c r="C396" s="4">
+      <c r="C396">
         <v>879.80997861796789</v>
       </c>
       <c r="E396" s="3"/>
@@ -6479,7 +6480,7 @@
       <c r="B397" t="s">
         <v>70</v>
       </c>
-      <c r="C397" s="4">
+      <c r="C397">
         <v>481.7769295899119</v>
       </c>
       <c r="E397" s="3"/>
@@ -6491,7 +6492,7 @@
       <c r="B398" t="s">
         <v>71</v>
       </c>
-      <c r="C398" s="4">
+      <c r="C398">
         <v>269.86344255679461</v>
       </c>
       <c r="E398" s="3"/>
@@ -6503,7 +6504,7 @@
       <c r="B399" t="s">
         <v>1</v>
       </c>
-      <c r="C399" s="4">
+      <c r="C399">
         <v>106.59930983884098</v>
       </c>
       <c r="E399" s="3"/>
@@ -6515,7 +6516,7 @@
       <c r="B400" t="s">
         <v>72</v>
       </c>
-      <c r="C400" s="4">
+      <c r="C400">
         <v>603.3931968314115</v>
       </c>
       <c r="E400" s="3"/>
@@ -6527,7 +6528,7 @@
       <c r="B401" t="s">
         <v>73</v>
       </c>
-      <c r="C401" s="4">
+      <c r="C401">
         <v>238.47713668020438</v>
       </c>
       <c r="E401" s="3"/>
@@ -6539,7 +6540,7 @@
       <c r="B402" t="s">
         <v>133</v>
       </c>
-      <c r="C402" s="4">
+      <c r="C402">
         <v>1601.1909504354824</v>
       </c>
       <c r="E402" s="3"/>
@@ -6551,7 +6552,7 @@
       <c r="B403" t="s">
         <v>74</v>
       </c>
-      <c r="C403" s="4">
+      <c r="C403">
         <v>636.58640701526576</v>
       </c>
       <c r="E403" s="3"/>
@@ -6563,7 +6564,7 @@
       <c r="B404" t="s">
         <v>75</v>
       </c>
-      <c r="C404" s="4">
+      <c r="C404">
         <v>1008.1977328300192</v>
       </c>
       <c r="E404" s="3"/>
@@ -6575,7 +6576,7 @@
       <c r="B405" t="s">
         <v>76</v>
       </c>
-      <c r="C405" s="4">
+      <c r="C405">
         <v>676.47873076282747</v>
       </c>
       <c r="E405" s="3"/>
@@ -6587,7 +6588,7 @@
       <c r="B406" t="s">
         <v>134</v>
       </c>
-      <c r="C406" s="4">
+      <c r="C406">
         <v>1683.196298644787</v>
       </c>
       <c r="E406" s="3"/>
@@ -6599,7 +6600,7 @@
       <c r="B407" t="s">
         <v>77</v>
       </c>
-      <c r="C407" s="4">
+      <c r="C407">
         <v>1114.2306721975945</v>
       </c>
       <c r="E407" s="3"/>
@@ -6611,7 +6612,7 @@
       <c r="B408" t="s">
         <v>78</v>
       </c>
-      <c r="C408" s="4">
+      <c r="C408">
         <v>1172.3817373219688</v>
       </c>
       <c r="E408" s="3"/>
@@ -6623,7 +6624,7 @@
       <c r="B409" t="s">
         <v>79</v>
       </c>
-      <c r="C409" s="4">
+      <c r="C409">
         <v>1698.1241695053361</v>
       </c>
       <c r="E409" s="3"/>
@@ -6635,7 +6636,7 @@
       <c r="B410" t="s">
         <v>80</v>
       </c>
-      <c r="C410" s="4">
+      <c r="C410">
         <v>966.58348519936146</v>
       </c>
       <c r="E410" s="3"/>
@@ -6647,7 +6648,7 @@
       <c r="B411" t="s">
         <v>81</v>
       </c>
-      <c r="C411" s="4">
+      <c r="C411">
         <v>57.106826330357059</v>
       </c>
       <c r="E411" s="3"/>
@@ -6659,7 +6660,7 @@
       <c r="B412" t="s">
         <v>82</v>
       </c>
-      <c r="C412" s="4">
+      <c r="C412">
         <v>57.781575542136721</v>
       </c>
       <c r="E412" s="3"/>
@@ -6671,7 +6672,7 @@
       <c r="B413" t="s">
         <v>135</v>
       </c>
-      <c r="C413" s="4">
+      <c r="C413">
         <v>529.90803950192003</v>
       </c>
       <c r="E413" s="3"/>
@@ -6683,7 +6684,7 @@
       <c r="B414" t="s">
         <v>136</v>
       </c>
-      <c r="C414" s="4">
+      <c r="C414">
         <v>753.77581858648534</v>
       </c>
       <c r="E414" s="3"/>
@@ -6695,7 +6696,7 @@
       <c r="B415" t="s">
         <v>83</v>
       </c>
-      <c r="C415" s="4">
+      <c r="C415">
         <v>1858.0891674780239</v>
       </c>
       <c r="E415" s="3"/>
@@ -6707,7 +6708,7 @@
       <c r="B416" t="s">
         <v>137</v>
       </c>
-      <c r="C416" s="4">
+      <c r="C416">
         <v>1233.6551179234411</v>
       </c>
       <c r="E416" s="3"/>
@@ -6719,7 +6720,7 @@
       <c r="B417" t="s">
         <v>84</v>
       </c>
-      <c r="C417" s="4">
+      <c r="C417">
         <v>507.05463881171568</v>
       </c>
       <c r="E417" s="3"/>
@@ -6731,7 +6732,7 @@
       <c r="B418" t="s">
         <v>85</v>
       </c>
-      <c r="C418" s="4">
+      <c r="C418">
         <v>232.86914653687487</v>
       </c>
       <c r="E418" s="3"/>
@@ -6743,7 +6744,7 @@
       <c r="B419" t="s">
         <v>86</v>
       </c>
-      <c r="C419" s="4">
+      <c r="C419">
         <v>535.92587085417983</v>
       </c>
       <c r="E419" s="3"/>
@@ -6755,7 +6756,7 @@
       <c r="B420" t="s">
         <v>87</v>
       </c>
-      <c r="C420" s="4">
+      <c r="C420">
         <v>1244.9465338657635</v>
       </c>
       <c r="E420" s="3"/>
@@ -6767,7 +6768,7 @@
       <c r="B421" t="s">
         <v>88</v>
       </c>
-      <c r="C421" s="4">
+      <c r="C421">
         <v>247.14134429167186</v>
       </c>
       <c r="E421" s="3"/>
@@ -6779,7 +6780,7 @@
       <c r="B422" t="s">
         <v>89</v>
       </c>
-      <c r="C422" s="4">
+      <c r="C422">
         <v>203.77673799656694</v>
       </c>
       <c r="E422" s="3"/>
@@ -6791,7 +6792,7 @@
       <c r="B423" t="s">
         <v>138</v>
       </c>
-      <c r="C423" s="4">
+      <c r="C423">
         <v>235.45716917009227</v>
       </c>
       <c r="E423" s="3"/>
@@ -6803,7 +6804,7 @@
       <c r="B424" t="s">
         <v>90</v>
       </c>
-      <c r="C424" s="4">
+      <c r="C424">
         <v>261.72641542278933</v>
       </c>
       <c r="E424" s="3"/>
@@ -6815,7 +6816,7 @@
       <c r="B425" t="s">
         <v>25</v>
       </c>
-      <c r="C425" s="4">
+      <c r="C425">
         <v>774.32998727141535</v>
       </c>
       <c r="E425" s="3"/>
@@ -6827,7 +6828,7 @@
       <c r="B426" t="s">
         <v>139</v>
       </c>
-      <c r="C426" s="4">
+      <c r="C426">
         <v>1118.7431021295995</v>
       </c>
       <c r="E426" s="3"/>
@@ -6839,7 +6840,7 @@
       <c r="B427" t="s">
         <v>140</v>
       </c>
-      <c r="C427" s="4">
+      <c r="C427">
         <v>99.8613505543575</v>
       </c>
       <c r="E427" s="3"/>
@@ -6851,7 +6852,7 @@
       <c r="B428" t="s">
         <v>141</v>
       </c>
-      <c r="C428" s="4">
+      <c r="C428">
         <v>400.83679258521954</v>
       </c>
       <c r="E428" s="3"/>
@@ -6863,7 +6864,7 @@
       <c r="B429" t="s">
         <v>91</v>
       </c>
-      <c r="C429" s="4">
+      <c r="C429">
         <v>1543.12413950207</v>
       </c>
       <c r="E429" s="3"/>
@@ -6875,7 +6876,7 @@
       <c r="B430" t="s">
         <v>142</v>
       </c>
-      <c r="C430" s="4">
+      <c r="C430">
         <v>1417.9280651296338</v>
       </c>
       <c r="E430" s="3"/>
@@ -6887,7 +6888,7 @@
       <c r="B431" t="s">
         <v>92</v>
       </c>
-      <c r="C431" s="4">
+      <c r="C431">
         <v>541.67804482218776</v>
       </c>
       <c r="E431" s="3"/>
@@ -6899,7 +6900,7 @@
       <c r="B432" t="s">
         <v>83</v>
       </c>
-      <c r="C432" s="4">
+      <c r="C432">
         <v>1858.0891674780239</v>
       </c>
       <c r="E432" s="3"/>
@@ -6911,7 +6912,7 @@
       <c r="B433" t="s">
         <v>93</v>
       </c>
-      <c r="C433" s="4">
+      <c r="C433">
         <v>1614.4729913928259</v>
       </c>
       <c r="E433" s="3"/>
@@ -6923,7 +6924,7 @@
       <c r="B434" t="s">
         <v>143</v>
       </c>
-      <c r="C434" s="4">
+      <c r="C434">
         <v>808.82809987455107</v>
       </c>
       <c r="E434" s="3"/>
@@ -6935,7 +6936,7 @@
       <c r="B435" t="s">
         <v>94</v>
       </c>
-      <c r="C435" s="4">
+      <c r="C435">
         <v>335.07395524282862</v>
       </c>
       <c r="E435" s="3"/>
@@ -6947,7 +6948,7 @@
       <c r="B436" t="s">
         <v>144</v>
       </c>
-      <c r="C436" s="4">
+      <c r="C436">
         <v>367.05284617454527</v>
       </c>
       <c r="E436" s="3"/>
@@ -6959,7 +6960,7 @@
       <c r="B437" t="s">
         <v>145</v>
       </c>
-      <c r="C437" s="4">
+      <c r="C437">
         <v>1713.3754762538372</v>
       </c>
       <c r="E437" s="3"/>
@@ -6971,7 +6972,7 @@
       <c r="B438" t="s">
         <v>95</v>
       </c>
-      <c r="C438" s="4">
+      <c r="C438">
         <v>862.6461629366645</v>
       </c>
       <c r="E438" s="3"/>
@@ -6983,7 +6984,7 @@
       <c r="B439" t="s">
         <v>96</v>
       </c>
-      <c r="C439" s="4">
+      <c r="C439">
         <v>427.35389817076401</v>
       </c>
       <c r="E439" s="3"/>
@@ -6995,7 +6996,7 @@
       <c r="B440" t="s">
         <v>97</v>
       </c>
-      <c r="C440" s="4">
+      <c r="C440">
         <v>690.70253375705715</v>
       </c>
       <c r="E440" s="3"/>
@@ -7007,7 +7008,7 @@
       <c r="B441" t="s">
         <v>146</v>
       </c>
-      <c r="C441" s="4">
+      <c r="C441">
         <v>898.51291812725231</v>
       </c>
       <c r="E441" s="3"/>
@@ -7019,7 +7020,7 @@
       <c r="B442" t="s">
         <v>10</v>
       </c>
-      <c r="C442" s="4">
+      <c r="C442">
         <v>1345.7678799316629</v>
       </c>
       <c r="E442" s="3"/>
@@ -7031,7 +7032,7 @@
       <c r="B443" t="s">
         <v>147</v>
       </c>
-      <c r="C443" s="4">
+      <c r="C443">
         <v>1182.475499354056</v>
       </c>
       <c r="E443" s="3"/>
@@ -7043,7 +7044,7 @@
       <c r="B444" t="s">
         <v>99</v>
       </c>
-      <c r="C444" s="4">
+      <c r="C444">
         <v>211.81142778330812</v>
       </c>
       <c r="E444" s="3"/>
@@ -7055,7 +7056,7 @@
       <c r="B445" t="s">
         <v>62</v>
       </c>
-      <c r="C445" s="4">
+      <c r="C445">
         <v>304.2477274964437</v>
       </c>
       <c r="E445" s="3"/>
@@ -7067,7 +7068,7 @@
       <c r="B446" t="s">
         <v>100</v>
       </c>
-      <c r="C446" s="4">
+      <c r="C446">
         <v>1455.8746436371093</v>
       </c>
       <c r="E446" s="3"/>
@@ -7079,7 +7080,7 @@
       <c r="B447" t="s">
         <v>148</v>
       </c>
-      <c r="C447" s="4">
+      <c r="C447">
         <v>832.3939319097866</v>
       </c>
       <c r="E447" s="3"/>
@@ -7091,7 +7092,7 @@
       <c r="B448" t="s">
         <v>149</v>
       </c>
-      <c r="C448" s="4">
+      <c r="C448">
         <v>749.02601552791441</v>
       </c>
       <c r="E448" s="3"/>
@@ -7103,7 +7104,7 @@
       <c r="B449" t="s">
         <v>150</v>
       </c>
-      <c r="C449" s="4">
+      <c r="C449">
         <v>832.44372508134506</v>
       </c>
       <c r="E449" s="3"/>
@@ -7115,7 +7116,7 @@
       <c r="B450" t="s">
         <v>101</v>
       </c>
-      <c r="C450" s="4">
+      <c r="C450">
         <v>363.01623442036555</v>
       </c>
       <c r="E450" s="3"/>
@@ -7127,7 +7128,7 @@
       <c r="B451" t="s">
         <v>151</v>
       </c>
-      <c r="C451" s="4">
+      <c r="C451">
         <v>127.1960771048962</v>
       </c>
       <c r="E451" s="3"/>
@@ -7139,7 +7140,7 @@
       <c r="B452" t="s">
         <v>102</v>
       </c>
-      <c r="C452" s="4">
+      <c r="C452">
         <v>366.35855434186544</v>
       </c>
       <c r="E452" s="3"/>
@@ -7151,7 +7152,7 @@
       <c r="B453" t="s">
         <v>103</v>
       </c>
-      <c r="C453" s="4">
+      <c r="C453">
         <v>1268.5490149726163</v>
       </c>
       <c r="E453" s="3"/>
@@ -7163,7 +7164,7 @@
       <c r="B454" t="s">
         <v>152</v>
       </c>
-      <c r="C454" s="4">
+      <c r="C454">
         <v>361.45397563439116</v>
       </c>
       <c r="E454" s="3"/>
@@ -7175,7 +7176,7 @@
       <c r="B455" t="s">
         <v>104</v>
       </c>
-      <c r="C455" s="4">
+      <c r="C455">
         <v>94.606317504974285</v>
       </c>
       <c r="E455" s="3"/>
@@ -7187,7 +7188,7 @@
       <c r="B456" t="s">
         <v>105</v>
       </c>
-      <c r="C456" s="4">
+      <c r="C456">
         <v>212.51507047672422</v>
       </c>
       <c r="E456" s="3"/>
@@ -7199,7 +7200,7 @@
       <c r="B457" t="s">
         <v>106</v>
       </c>
-      <c r="C457" s="4">
+      <c r="C457">
         <v>93.138895021374537</v>
       </c>
       <c r="E457" s="3"/>
@@ -7211,7 +7212,7 @@
       <c r="B458" t="s">
         <v>107</v>
       </c>
-      <c r="C458" s="4">
+      <c r="C458">
         <v>42.629103117245421</v>
       </c>
       <c r="E458" s="3"/>
@@ -7223,7 +7224,7 @@
       <c r="B459" t="s">
         <v>108</v>
       </c>
-      <c r="C459" s="4">
+      <c r="C459">
         <v>881.97012301463485</v>
       </c>
       <c r="E459" s="3"/>
@@ -7235,7 +7236,7 @@
       <c r="B460" t="s">
         <v>153</v>
       </c>
-      <c r="C460" s="4">
+      <c r="C460">
         <v>214.97246899183432</v>
       </c>
       <c r="E460" s="3"/>
@@ -7247,7 +7248,7 @@
       <c r="B461" t="s">
         <v>109</v>
       </c>
-      <c r="C461" s="4">
+      <c r="C461">
         <v>92.687440468983127</v>
       </c>
       <c r="E461" s="3"/>
@@ -7259,7 +7260,7 @@
       <c r="B462" t="s">
         <v>154</v>
       </c>
-      <c r="C462" s="4">
+      <c r="C462">
         <v>1181.8798577183375</v>
       </c>
       <c r="E462" s="3"/>
@@ -7271,7 +7272,7 @@
       <c r="B463" t="s">
         <v>155</v>
       </c>
-      <c r="C463" s="4">
+      <c r="C463">
         <v>1314.1332360146855</v>
       </c>
       <c r="E463" s="3"/>
@@ -7283,7 +7284,7 @@
       <c r="B464" t="s">
         <v>110</v>
       </c>
-      <c r="C464" s="4">
+      <c r="C464">
         <v>2292.0065080158088</v>
       </c>
       <c r="E464" s="3"/>
@@ -7295,7 +7296,7 @@
       <c r="B465" t="s">
         <v>111</v>
       </c>
-      <c r="C465" s="4">
+      <c r="C465">
         <v>69.869123092669753</v>
       </c>
       <c r="E465" s="3"/>
@@ -7307,7 +7308,7 @@
       <c r="B466" t="s">
         <v>112</v>
       </c>
-      <c r="C466" s="4">
+      <c r="C466">
         <v>87.268012771614337</v>
       </c>
       <c r="E466" s="3"/>
@@ -7319,7 +7320,7 @@
       <c r="B467" t="s">
         <v>156</v>
       </c>
-      <c r="C467" s="4">
+      <c r="C467">
         <v>362.29196370835035</v>
       </c>
       <c r="E467" s="3"/>
@@ -7331,7 +7332,7 @@
       <c r="B468" t="s">
         <v>157</v>
       </c>
-      <c r="C468" s="4">
+      <c r="C468">
         <v>230.19362742792055</v>
       </c>
       <c r="E468" s="3"/>
@@ -7343,7 +7344,7 @@
       <c r="B469" t="s">
         <v>61</v>
       </c>
-      <c r="C469" s="4">
+      <c r="C469">
         <v>900.45029954325207</v>
       </c>
       <c r="E469" s="3"/>
@@ -7355,7 +7356,7 @@
       <c r="B470" t="s">
         <v>158</v>
       </c>
-      <c r="C470" s="4">
+      <c r="C470">
         <v>1040.7649316737686</v>
       </c>
       <c r="E470" s="3"/>
@@ -7367,7 +7368,7 @@
       <c r="B471" t="s">
         <v>113</v>
       </c>
-      <c r="C471" s="4">
+      <c r="C471">
         <v>739.75254003570114</v>
       </c>
       <c r="E471" s="3"/>
@@ -7379,7 +7380,7 @@
       <c r="B472" t="s">
         <v>114</v>
       </c>
-      <c r="C472" s="4">
+      <c r="C472">
         <v>780.21139630808636</v>
       </c>
       <c r="E472" s="3"/>
@@ -7391,7 +7392,7 @@
       <c r="B473" t="s">
         <v>115</v>
       </c>
-      <c r="C473" s="4">
+      <c r="C473">
         <v>61.145660885545034</v>
       </c>
       <c r="E473" s="3"/>
@@ -7403,7 +7404,7 @@
       <c r="B474" t="s">
         <v>159</v>
       </c>
-      <c r="C474" s="4">
+      <c r="C474">
         <v>249.30188927117325</v>
       </c>
       <c r="E474" s="3"/>
@@ -7415,7 +7416,7 @@
       <c r="B475" t="s">
         <v>116</v>
       </c>
-      <c r="C475" s="4">
+      <c r="C475">
         <v>1006.7255892792932</v>
       </c>
       <c r="E475" s="3"/>
@@ -7427,7 +7428,7 @@
       <c r="B476" t="s">
         <v>117</v>
       </c>
-      <c r="C476" s="4">
+      <c r="C476">
         <v>1178.3535843287802</v>
       </c>
       <c r="E476" s="3"/>
@@ -7439,7 +7440,7 @@
       <c r="B477" t="s">
         <v>98</v>
       </c>
-      <c r="C477" s="4">
+      <c r="C477">
         <v>670.52024114618996</v>
       </c>
       <c r="E477" s="3"/>
@@ -15408,7 +15409,7 @@
         <v>17</v>
       </c>
       <c r="C1090">
-        <v>5863.5424001638939</v>
+        <v>1352.4171849501404</v>
       </c>
       <c r="D1090" s="4"/>
       <c r="E1090" s="3"/>
@@ -15421,7 +15422,7 @@
         <v>18</v>
       </c>
       <c r="C1091">
-        <v>4619.5444506453896</v>
+        <v>1093.1813280222345</v>
       </c>
       <c r="D1091" s="4"/>
       <c r="E1091" s="3"/>
@@ -15434,7 +15435,7 @@
         <v>19</v>
       </c>
       <c r="C1092">
-        <v>4678.9960655019077</v>
+        <v>801.4826088306354</v>
       </c>
       <c r="D1092" s="4"/>
       <c r="E1092" s="3"/>
@@ -15447,7 +15448,7 @@
         <v>20</v>
       </c>
       <c r="C1093">
-        <v>4779.9585212943484</v>
+        <v>858.06951780590475</v>
       </c>
       <c r="D1093" s="4"/>
       <c r="E1093" s="3"/>
@@ -15460,7 +15461,7 @@
         <v>118</v>
       </c>
       <c r="C1094">
-        <v>4580.6478659776303</v>
+        <v>858.13217853017784</v>
       </c>
       <c r="D1094" s="4"/>
       <c r="E1094" s="3"/>
@@ -15473,7 +15474,7 @@
         <v>3</v>
       </c>
       <c r="C1095">
-        <v>6450.6687783320531</v>
+        <v>994.058120631625</v>
       </c>
       <c r="D1095" s="4"/>
       <c r="E1095" s="3"/>
@@ -15486,7 +15487,7 @@
         <v>119</v>
       </c>
       <c r="C1096">
-        <v>5586.1063123770409</v>
+        <v>904.19022764259569</v>
       </c>
       <c r="D1096" s="4"/>
       <c r="E1096" s="3"/>
@@ -15499,7 +15500,7 @@
         <v>21</v>
       </c>
       <c r="C1097">
-        <v>5841.2239000503732</v>
+        <v>981.36886731313746</v>
       </c>
       <c r="D1097" s="4"/>
       <c r="E1097" s="3"/>
@@ -15512,7 +15513,7 @@
         <v>22</v>
       </c>
       <c r="C1098">
-        <v>5446.5410563232563</v>
+        <v>1357.3164973805763</v>
       </c>
       <c r="D1098" s="4"/>
       <c r="E1098" s="3"/>
@@ -15525,7 +15526,7 @@
         <v>120</v>
       </c>
       <c r="C1099">
-        <v>4798.7326909036683</v>
+        <v>1272.2367403664446</v>
       </c>
       <c r="D1099" s="4"/>
       <c r="E1099" s="3"/>
@@ -15538,7 +15539,7 @@
         <v>6</v>
       </c>
       <c r="C1100">
-        <v>5642.4625318166991</v>
+        <v>2042.8419783235697</v>
       </c>
       <c r="D1100" s="4"/>
       <c r="E1100" s="3"/>
@@ -15551,7 +15552,7 @@
         <v>23</v>
       </c>
       <c r="C1101">
-        <v>5410.8192599520453</v>
+        <v>2410.1456141581025</v>
       </c>
       <c r="D1101" s="4"/>
       <c r="E1101" s="3"/>
@@ -15564,7 +15565,7 @@
         <v>121</v>
       </c>
       <c r="C1102">
-        <v>6731.949322467407</v>
+        <v>1306.3888724029168</v>
       </c>
       <c r="D1102" s="4"/>
       <c r="E1102" s="3"/>
@@ -15577,7 +15578,7 @@
         <v>24</v>
       </c>
       <c r="C1103">
-        <v>5267.4080295563617</v>
+        <v>144.46981916701975</v>
       </c>
       <c r="D1103" s="4"/>
       <c r="E1103" s="3"/>
@@ -15590,7 +15591,7 @@
         <v>122</v>
       </c>
       <c r="C1104">
-        <v>4617.0447081986113</v>
+        <v>784.43953841320172</v>
       </c>
       <c r="D1104" s="4"/>
       <c r="E1104" s="3"/>
@@ -15603,7 +15604,7 @@
         <v>26</v>
       </c>
       <c r="C1105">
-        <v>4658.3391639374868</v>
+        <v>784.43953841320172</v>
       </c>
       <c r="D1105" s="4"/>
       <c r="E1105" s="3"/>
@@ -15616,7 +15617,7 @@
         <v>27</v>
       </c>
       <c r="C1106">
-        <v>5760.0616033343631</v>
+        <v>1024.5947146504047</v>
       </c>
       <c r="D1106" s="4"/>
       <c r="E1106" s="3"/>
@@ -15629,7 +15630,7 @@
         <v>28</v>
       </c>
       <c r="C1107">
-        <v>5238.2917171884246</v>
+        <v>1232.8229272836868</v>
       </c>
       <c r="D1107" s="4"/>
       <c r="E1107" s="3"/>
@@ -15642,7 +15643,7 @@
         <v>29</v>
       </c>
       <c r="C1108">
-        <v>4593.7637517916073</v>
+        <v>2095.4605518442445</v>
       </c>
       <c r="D1108" s="4"/>
       <c r="E1108" s="3"/>
@@ -15655,7 +15656,7 @@
         <v>123</v>
       </c>
       <c r="C1109">
-        <v>4600.788682513753</v>
+        <v>760.68643612870483</v>
       </c>
       <c r="D1109" s="4"/>
       <c r="E1109" s="3"/>
@@ -15668,7 +15669,7 @@
         <v>124</v>
       </c>
       <c r="C1110">
-        <v>6113.8366657597053</v>
+        <v>2427.3519572618266</v>
       </c>
       <c r="D1110" s="4"/>
       <c r="E1110" s="3"/>
@@ -15681,7 +15682,7 @@
         <v>30</v>
       </c>
       <c r="C1111">
-        <v>5140.439569142598</v>
+        <v>2102.6302186001408</v>
       </c>
       <c r="D1111" s="4"/>
       <c r="E1111" s="3"/>
@@ -15694,7 +15695,7 @@
         <v>31</v>
       </c>
       <c r="C1112">
-        <v>5747.9365876050833</v>
+        <v>2008.3559621067948</v>
       </c>
       <c r="D1112" s="4"/>
       <c r="E1112" s="3"/>
@@ -15707,7 +15708,7 @@
         <v>32</v>
       </c>
       <c r="C1113">
-        <v>4740.9889625858705</v>
+        <v>145.64154173610399</v>
       </c>
       <c r="D1113" s="4"/>
       <c r="E1113" s="3"/>
@@ -15720,7 +15721,7 @@
         <v>33</v>
       </c>
       <c r="C1114">
-        <v>6035.5794876280634</v>
+        <v>372.68917951321191</v>
       </c>
       <c r="D1114" s="4"/>
       <c r="E1114" s="3"/>
@@ -15733,7 +15734,7 @@
         <v>34</v>
       </c>
       <c r="C1115">
-        <v>6844.4595539365346</v>
+        <v>1056.2997936720149</v>
       </c>
       <c r="D1115" s="4"/>
       <c r="E1115" s="3"/>
@@ -15746,7 +15747,7 @@
         <v>35</v>
       </c>
       <c r="C1116">
-        <v>6015.7161666088277</v>
+        <v>1083.7101960482214</v>
       </c>
       <c r="D1116" s="4"/>
       <c r="E1116" s="3"/>
@@ -15759,7 +15760,7 @@
         <v>36</v>
       </c>
       <c r="C1117">
-        <v>5835.1784710938682</v>
+        <v>2090.1628661570016</v>
       </c>
       <c r="D1117" s="4"/>
       <c r="E1117" s="3"/>
@@ -15772,7 +15773,7 @@
         <v>37</v>
       </c>
       <c r="C1118">
-        <v>5662.5156277987171</v>
+        <v>2361.2044006978072</v>
       </c>
       <c r="D1118" s="4"/>
       <c r="E1118" s="3"/>
@@ -15785,7 +15786,7 @@
         <v>38</v>
       </c>
       <c r="C1119">
-        <v>6733.2672824880292</v>
+        <v>647.58868235954492</v>
       </c>
       <c r="D1119" s="4"/>
       <c r="E1119" s="3"/>
@@ -15798,7 +15799,7 @@
         <v>39</v>
       </c>
       <c r="C1120">
-        <v>5753.3910512356688</v>
+        <v>1339.9600132113685</v>
       </c>
       <c r="D1120" s="4"/>
       <c r="E1120" s="3"/>
@@ -15811,7 +15812,7 @@
         <v>40</v>
       </c>
       <c r="C1121">
-        <v>6260.0756724711055</v>
+        <v>1773.7063636929081</v>
       </c>
       <c r="D1121" s="4"/>
       <c r="E1121" s="3"/>
@@ -15824,7 +15825,7 @@
         <v>41</v>
       </c>
       <c r="C1122">
-        <v>5408.0747620127249</v>
+        <v>871.70512887893813</v>
       </c>
       <c r="D1122" s="4"/>
       <c r="E1122" s="3"/>
@@ -15837,7 +15838,7 @@
         <v>9</v>
       </c>
       <c r="C1123">
-        <v>7424.5367279949232</v>
+        <v>1886.5902349059079</v>
       </c>
       <c r="D1123" s="4"/>
       <c r="E1123" s="3"/>
@@ -15850,7 +15851,7 @@
         <v>42</v>
       </c>
       <c r="C1124">
-        <v>5557.0943292618931</v>
+        <v>2081.4134734350719</v>
       </c>
       <c r="D1124" s="4"/>
       <c r="E1124" s="3"/>
@@ -15863,7 +15864,7 @@
         <v>125</v>
       </c>
       <c r="C1125">
-        <v>5728.4352892762472</v>
+        <v>2434.6437857070573</v>
       </c>
       <c r="D1125" s="4"/>
       <c r="E1125" s="3"/>
@@ -15876,7 +15877,7 @@
         <v>43</v>
       </c>
       <c r="C1126">
-        <v>4597.7742067976696</v>
+        <v>584.6022645384819</v>
       </c>
       <c r="D1126" s="4"/>
       <c r="E1126" s="3"/>
@@ -15889,7 +15890,7 @@
         <v>44</v>
       </c>
       <c r="C1127">
-        <v>4720.4115697844391</v>
+        <v>1313.2504868971328</v>
       </c>
       <c r="D1127" s="4"/>
       <c r="E1127" s="3"/>
@@ -15902,7 +15903,7 @@
         <v>45</v>
       </c>
       <c r="C1128">
-        <v>6000.2598238388618</v>
+        <v>1283.8021871614653</v>
       </c>
       <c r="D1128" s="4"/>
       <c r="E1128" s="3"/>
@@ -15915,7 +15916,7 @@
         <v>126</v>
       </c>
       <c r="C1129">
-        <v>6306.2370210411564</v>
+        <v>304.29933302658287</v>
       </c>
       <c r="D1129" s="4"/>
       <c r="E1129" s="3"/>
@@ -15928,7 +15929,7 @@
         <v>127</v>
       </c>
       <c r="C1130">
-        <v>5781.8146856880803</v>
+        <v>1100.1384809323467</v>
       </c>
       <c r="D1130" s="4"/>
       <c r="E1130" s="3"/>
@@ -15941,7 +15942,7 @@
         <v>46</v>
       </c>
       <c r="C1131">
-        <v>5489.8600299365989</v>
+        <v>586.88289275064903</v>
       </c>
       <c r="D1131" s="4"/>
       <c r="E1131" s="3"/>
@@ -15954,7 +15955,7 @@
         <v>47</v>
       </c>
       <c r="C1132">
-        <v>5599.8091783048767</v>
+        <v>1101.157229289252</v>
       </c>
       <c r="D1132" s="4"/>
       <c r="E1132" s="3"/>
@@ -15967,7 +15968,7 @@
         <v>48</v>
       </c>
       <c r="C1133">
-        <v>5445.0475068532714</v>
+        <v>1245.0638584219412</v>
       </c>
       <c r="D1133" s="4"/>
       <c r="E1133" s="3"/>
@@ -15980,7 +15981,7 @@
         <v>128</v>
       </c>
       <c r="C1134">
-        <v>6302.4899729826875</v>
+        <v>795.91942377877433</v>
       </c>
       <c r="D1134" s="4"/>
       <c r="E1134" s="3"/>
@@ -15993,7 +15994,7 @@
         <v>49</v>
       </c>
       <c r="C1135">
-        <v>5365.4184567469501</v>
+        <v>1057.264926648352</v>
       </c>
       <c r="D1135" s="4"/>
       <c r="E1135" s="3"/>
@@ -16006,7 +16007,7 @@
         <v>50</v>
       </c>
       <c r="C1136">
-        <v>5872.8264028484364</v>
+        <v>2114.7047704159595</v>
       </c>
       <c r="D1136" s="4"/>
       <c r="E1136" s="3"/>
@@ -16019,7 +16020,7 @@
         <v>51</v>
       </c>
       <c r="C1137">
-        <v>7455.0053597005581</v>
+        <v>2342.0043926429476</v>
       </c>
       <c r="D1137" s="4"/>
       <c r="E1137" s="3"/>
@@ -16032,7 +16033,7 @@
         <v>52</v>
       </c>
       <c r="C1138">
-        <v>5482.3375869628608</v>
+        <v>719.56919914588059</v>
       </c>
       <c r="D1138" s="4"/>
       <c r="E1138" s="3"/>
@@ -16045,7 +16046,7 @@
         <v>16</v>
       </c>
       <c r="C1139">
-        <v>4699.5013938526308</v>
+        <v>992.14361701232008</v>
       </c>
       <c r="D1139" s="4"/>
       <c r="E1139" s="3"/>
@@ -16058,7 +16059,7 @@
         <v>53</v>
       </c>
       <c r="C1140">
-        <v>4474.8450065425923</v>
+        <v>813.99095694016466</v>
       </c>
       <c r="D1140" s="4"/>
       <c r="E1140" s="3"/>
@@ -16071,7 +16072,7 @@
         <v>54</v>
       </c>
       <c r="C1141">
-        <v>6068.4279219373147</v>
+        <v>815.9521688932814</v>
       </c>
       <c r="D1141" s="4"/>
       <c r="E1141" s="3"/>
@@ -16084,7 +16085,7 @@
         <v>55</v>
       </c>
       <c r="C1142">
-        <v>4580.0944006448426</v>
+        <v>1018.2300080972932</v>
       </c>
       <c r="D1142" s="4"/>
       <c r="E1142" s="3"/>
@@ -16097,7 +16098,7 @@
         <v>56</v>
       </c>
       <c r="C1143">
-        <v>5238.756659540195</v>
+        <v>234.41416320476114</v>
       </c>
       <c r="D1143" s="4"/>
       <c r="E1143" s="3"/>
@@ -16110,7 +16111,7 @@
         <v>57</v>
       </c>
       <c r="C1144">
-        <v>7525.7555887960052</v>
+        <v>442.81579229027187</v>
       </c>
       <c r="D1144" s="4"/>
       <c r="E1144" s="3"/>
@@ -16123,7 +16124,7 @@
         <v>58</v>
       </c>
       <c r="C1145">
-        <v>5153.2176419063144</v>
+        <v>554.54753226905677</v>
       </c>
       <c r="D1145" s="4"/>
       <c r="E1145" s="3"/>
@@ -16136,7 +16137,7 @@
         <v>59</v>
       </c>
       <c r="C1146">
-        <v>5087.1291227423426</v>
+        <v>559.57577027254115</v>
       </c>
       <c r="D1146" s="4"/>
       <c r="E1146" s="3"/>
@@ -16149,7 +16150,7 @@
         <v>15</v>
       </c>
       <c r="C1147">
-        <v>5010.9118826918857</v>
+        <v>1478.6122010914457</v>
       </c>
       <c r="D1147" s="4"/>
       <c r="E1147" s="3"/>
@@ -16162,7 +16163,7 @@
         <v>129</v>
       </c>
       <c r="C1148">
-        <v>4659.6265265678339</v>
+        <v>1265.4717645699823</v>
       </c>
       <c r="D1148" s="4"/>
       <c r="E1148" s="3"/>
@@ -16175,7 +16176,7 @@
         <v>60</v>
       </c>
       <c r="C1149">
-        <v>4809.3739662488588</v>
+        <v>998.19596934147557</v>
       </c>
       <c r="D1149" s="4"/>
       <c r="E1149" s="3"/>
@@ -16188,7 +16189,7 @@
         <v>130</v>
       </c>
       <c r="C1150">
-        <v>5945.8069272011599</v>
+        <v>2437.73791905794</v>
       </c>
       <c r="D1150" s="4"/>
       <c r="E1150" s="3"/>
@@ -16201,7 +16202,7 @@
         <v>62</v>
       </c>
       <c r="C1151">
-        <v>5446.617376125686</v>
+        <v>1380.904529049146</v>
       </c>
       <c r="D1151" s="4"/>
       <c r="E1151" s="3"/>
@@ -16214,7 +16215,7 @@
         <v>131</v>
       </c>
       <c r="C1152">
-        <v>4499.0201529129945</v>
+        <v>1301.8154617614239</v>
       </c>
       <c r="D1152" s="4"/>
       <c r="E1152" s="3"/>
@@ -16227,7 +16228,7 @@
         <v>63</v>
       </c>
       <c r="C1153">
-        <v>5685.0131002658045</v>
+        <v>920.25204784179698</v>
       </c>
       <c r="D1153" s="4"/>
       <c r="E1153" s="3"/>
@@ -16240,7 +16241,7 @@
         <v>64</v>
       </c>
       <c r="C1154">
-        <v>6652.7959381912879</v>
+        <v>906.96401405104132</v>
       </c>
       <c r="D1154" s="4"/>
       <c r="E1154" s="3"/>
@@ -16253,7 +16254,7 @@
         <v>65</v>
       </c>
       <c r="C1155">
-        <v>5497.5148756227709</v>
+        <v>1145.3265889606844</v>
       </c>
       <c r="D1155" s="4"/>
       <c r="E1155" s="3"/>
@@ -16266,7 +16267,7 @@
         <v>12</v>
       </c>
       <c r="C1156">
-        <v>5387.0968049159219</v>
+        <v>2098.6616154698277</v>
       </c>
       <c r="D1156" s="4"/>
       <c r="E1156" s="3"/>
@@ -16279,7 +16280,7 @@
         <v>66</v>
       </c>
       <c r="C1157">
-        <v>5822.8903320886384</v>
+        <v>1087.1828859147042</v>
       </c>
       <c r="D1157" s="4"/>
       <c r="E1157" s="3"/>
@@ -16292,7 +16293,7 @@
         <v>67</v>
       </c>
       <c r="C1158">
-        <v>5680.2933793395841</v>
+        <v>947.00433799798327</v>
       </c>
       <c r="D1158" s="4"/>
       <c r="E1158" s="3"/>
@@ -16305,7 +16306,7 @@
         <v>132</v>
       </c>
       <c r="C1159">
-        <v>7198.0208065624038</v>
+        <v>1105.6757663280812</v>
       </c>
       <c r="D1159" s="4"/>
       <c r="E1159" s="3"/>
@@ -16318,7 +16319,7 @@
         <v>68</v>
       </c>
       <c r="C1160">
-        <v>4722.7653154454138</v>
+        <v>226.82870762033988</v>
       </c>
       <c r="D1160" s="4"/>
       <c r="E1160" s="3"/>
@@ -16331,7 +16332,7 @@
         <v>69</v>
       </c>
       <c r="C1161">
-        <v>4388.4658792433911</v>
+        <v>1173.3808285508621</v>
       </c>
       <c r="D1161" s="4"/>
       <c r="E1161" s="3"/>
@@ -16344,7 +16345,7 @@
         <v>70</v>
       </c>
       <c r="C1162">
-        <v>5561.3567073351105</v>
+        <v>835.92793456549657</v>
       </c>
       <c r="D1162" s="4"/>
       <c r="E1162" s="3"/>
@@ -16357,7 +16358,7 @@
         <v>71</v>
       </c>
       <c r="C1163">
-        <v>5497.5397121878477</v>
+        <v>1304.4316891432522</v>
       </c>
       <c r="D1163" s="4"/>
       <c r="E1163" s="3"/>
@@ -16370,7 +16371,7 @@
         <v>1</v>
       </c>
       <c r="C1164">
-        <v>5276.6882008811845</v>
+        <v>409.55741555980148</v>
       </c>
       <c r="D1164" s="4"/>
       <c r="E1164" s="3"/>
@@ -16383,7 +16384,7 @@
         <v>72</v>
       </c>
       <c r="C1165">
-        <v>5712.3079131863651</v>
+        <v>2151.5773157019089</v>
       </c>
       <c r="D1165" s="4"/>
       <c r="E1165" s="3"/>
@@ -16396,7 +16397,7 @@
         <v>73</v>
       </c>
       <c r="C1166">
-        <v>5337.3162506838462</v>
+        <v>1068.2598787941465</v>
       </c>
       <c r="D1166" s="4"/>
       <c r="E1166" s="3"/>
@@ -16409,7 +16410,7 @@
         <v>133</v>
       </c>
       <c r="C1167">
-        <v>6811.1317169823405</v>
+        <v>1266.870682206918</v>
       </c>
       <c r="D1167" s="4"/>
       <c r="E1167" s="3"/>
@@ -16422,7 +16423,7 @@
         <v>74</v>
       </c>
       <c r="C1168">
-        <v>4747.7575527941954</v>
+        <v>1800.5953415671711</v>
       </c>
       <c r="D1168" s="4"/>
       <c r="E1168" s="3"/>
@@ -16435,7 +16436,7 @@
         <v>75</v>
       </c>
       <c r="C1169">
-        <v>4812.1413850016734</v>
+        <v>943.528374090189</v>
       </c>
       <c r="D1169" s="4"/>
       <c r="E1169" s="3"/>
@@ -16448,7 +16449,7 @@
         <v>76</v>
       </c>
       <c r="C1170">
-        <v>5836.7156222826188</v>
+        <v>1022.3549603533987</v>
       </c>
       <c r="D1170" s="4"/>
       <c r="E1170" s="3"/>
@@ -16461,7 +16462,7 @@
         <v>134</v>
       </c>
       <c r="C1171">
-        <v>6913.571849406324</v>
+        <v>1062.0115842892515</v>
       </c>
       <c r="D1171" s="4"/>
       <c r="E1171" s="3"/>
@@ -16474,7 +16475,7 @@
         <v>77</v>
       </c>
       <c r="C1172">
-        <v>6192.7985690937858</v>
+        <v>695.79624223686255</v>
       </c>
       <c r="D1172" s="4"/>
       <c r="E1172" s="3"/>
@@ -16487,7 +16488,7 @@
         <v>78</v>
       </c>
       <c r="C1173">
-        <v>4372.9850801374296</v>
+        <v>1331.6679001422292</v>
       </c>
       <c r="D1173" s="4"/>
       <c r="E1173" s="3"/>
@@ -16500,7 +16501,7 @@
         <v>79</v>
       </c>
       <c r="C1174">
-        <v>6933.5680487199306</v>
+        <v>333.45597040506556</v>
       </c>
       <c r="D1174" s="4"/>
       <c r="E1174" s="3"/>
@@ -16513,7 +16514,7 @@
         <v>80</v>
       </c>
       <c r="C1175">
-        <v>6082.4815849597453</v>
+        <v>377.20214010276862</v>
       </c>
       <c r="D1175" s="4"/>
       <c r="E1175" s="3"/>
@@ -16526,7 +16527,7 @@
         <v>81</v>
       </c>
       <c r="C1176">
-        <v>5264.084233120996</v>
+        <v>736.91222826299895</v>
       </c>
       <c r="D1176" s="4"/>
       <c r="E1176" s="3"/>
@@ -16539,7 +16540,7 @@
         <v>82</v>
       </c>
       <c r="C1177">
-        <v>5203.6577098649987</v>
+        <v>1141.8053518818911</v>
       </c>
       <c r="D1177" s="4"/>
       <c r="E1177" s="3"/>
@@ -16552,7 +16553,7 @@
         <v>135</v>
       </c>
       <c r="C1178">
-        <v>5638.1678361350805</v>
+        <v>1617.192456287939</v>
       </c>
       <c r="D1178" s="4"/>
       <c r="E1178" s="3"/>
@@ -16565,7 +16566,7 @@
         <v>136</v>
       </c>
       <c r="C1179">
-        <v>5879.61875966766</v>
+        <v>838.75945887903845</v>
       </c>
       <c r="D1179" s="4"/>
       <c r="E1179" s="3"/>
@@ -16578,7 +16579,7 @@
         <v>83</v>
       </c>
       <c r="C1180">
-        <v>7095.7380700737685</v>
+        <v>1272.5596843907747</v>
       </c>
       <c r="D1180" s="4"/>
       <c r="E1180" s="3"/>
@@ -16591,7 +16592,7 @@
         <v>137</v>
       </c>
       <c r="C1181">
-        <v>6453.0505578227258</v>
+        <v>2059.4868912429733</v>
       </c>
       <c r="D1181" s="4"/>
       <c r="E1181" s="3"/>
@@ -16604,7 +16605,7 @@
         <v>84</v>
       </c>
       <c r="C1182">
-        <v>5745.342511550326</v>
+        <v>1885.5796344379203</v>
       </c>
       <c r="D1182" s="4"/>
       <c r="E1182" s="3"/>
@@ -16617,7 +16618,7 @@
         <v>85</v>
       </c>
       <c r="C1183">
-        <v>5094.0472403848289</v>
+        <v>1097.7751222129748</v>
       </c>
       <c r="D1183" s="4"/>
       <c r="E1183" s="3"/>
@@ -16630,7 +16631,7 @@
         <v>86</v>
       </c>
       <c r="C1184">
-        <v>4767.3349686655247</v>
+        <v>1544.0098127444587</v>
       </c>
       <c r="D1184" s="4"/>
       <c r="E1184" s="3"/>
@@ -16643,7 +16644,7 @@
         <v>87</v>
       </c>
       <c r="C1185">
-        <v>6430.8163389711735</v>
+        <v>2417.6299992674881</v>
       </c>
       <c r="D1185" s="4"/>
       <c r="E1185" s="3"/>
@@ -16656,7 +16657,7 @@
         <v>88</v>
       </c>
       <c r="C1186">
-        <v>5247.2000807884351</v>
+        <v>1382.0746692345422</v>
       </c>
       <c r="D1186" s="4"/>
       <c r="E1186" s="3"/>
@@ -16669,7 +16670,7 @@
         <v>89</v>
       </c>
       <c r="C1187">
-        <v>5330.5170017526098</v>
+        <v>2139.7140612497251</v>
       </c>
       <c r="D1187" s="4"/>
       <c r="E1187" s="3"/>
@@ -16682,7 +16683,7 @@
         <v>138</v>
       </c>
       <c r="C1188">
-        <v>5473.4562144032479</v>
+        <v>1374.0208235265336</v>
       </c>
       <c r="D1188" s="4"/>
       <c r="E1188" s="3"/>
@@ -16695,7 +16696,7 @@
         <v>90</v>
       </c>
       <c r="C1189">
-        <v>5299.5117156649139</v>
+        <v>1659.6147486054072</v>
       </c>
       <c r="D1189" s="4"/>
       <c r="E1189" s="3"/>
@@ -16708,7 +16709,7 @@
         <v>25</v>
       </c>
       <c r="C1190">
-        <v>4688.3246735339899</v>
+        <v>875.30744795035764</v>
       </c>
       <c r="D1190" s="4"/>
       <c r="E1190" s="3"/>
@@ -16721,7 +16722,7 @@
         <v>139</v>
       </c>
       <c r="C1191">
-        <v>6193.9206756179992</v>
+        <v>652.3372837832494</v>
       </c>
       <c r="D1191" s="4"/>
       <c r="E1191" s="3"/>
@@ -16734,7 +16735,7 @@
         <v>140</v>
       </c>
       <c r="C1192">
-        <v>5144.8793719670448</v>
+        <v>1110.9335460897082</v>
       </c>
       <c r="D1192" s="4"/>
       <c r="E1192" s="3"/>
@@ -16747,7 +16748,7 @@
         <v>141</v>
       </c>
       <c r="C1193">
-        <v>5605.0948003062258</v>
+        <v>1228.2677534950544</v>
       </c>
       <c r="D1193" s="4"/>
       <c r="E1193" s="3"/>
@@ -16760,7 +16761,7 @@
         <v>91</v>
       </c>
       <c r="C1194">
-        <v>6772.1990259518898</v>
+        <v>1246.822239262325</v>
       </c>
       <c r="D1194" s="4"/>
       <c r="E1194" s="3"/>
@@ -16773,7 +16774,7 @@
         <v>142</v>
       </c>
       <c r="C1195">
-        <v>6648.5628031220158</v>
+        <v>1344.3535159929954</v>
       </c>
       <c r="D1195" s="4"/>
       <c r="E1195" s="3"/>
@@ -16786,7 +16787,7 @@
         <v>92</v>
       </c>
       <c r="C1196">
-        <v>5595.7254341339194</v>
+        <v>1127.2293287979201</v>
       </c>
       <c r="D1196" s="4"/>
       <c r="E1196" s="3"/>
@@ -16799,7 +16800,7 @@
         <v>83</v>
       </c>
       <c r="C1197">
-        <v>7095.7380700737685</v>
+        <v>1014.7871558185151</v>
       </c>
       <c r="D1197" s="4"/>
       <c r="E1197" s="3"/>
@@ -16812,7 +16813,7 @@
         <v>93</v>
       </c>
       <c r="C1198">
-        <v>6850.5326175293003</v>
+        <v>1016.8458216228283</v>
       </c>
       <c r="D1198" s="4"/>
       <c r="E1198" s="3"/>
@@ -16825,7 +16826,7 @@
         <v>143</v>
       </c>
       <c r="C1199">
-        <v>6047.0701695838834</v>
+        <v>1028.7341853888706</v>
       </c>
       <c r="D1199" s="4"/>
       <c r="E1199" s="3"/>
@@ -16838,7 +16839,7 @@
         <v>94</v>
       </c>
       <c r="C1200">
-        <v>5513.1087793713832</v>
+        <v>951.38565192609315</v>
       </c>
       <c r="D1200" s="4"/>
       <c r="E1200" s="3"/>
@@ -16851,7 +16852,7 @@
         <v>144</v>
       </c>
       <c r="C1201">
-        <v>5556.0376150329412</v>
+        <v>1366.7259824205298</v>
       </c>
       <c r="D1201" s="4"/>
       <c r="E1201" s="3"/>
@@ -16864,7 +16865,7 @@
         <v>145</v>
       </c>
       <c r="C1202">
-        <v>6951.6391181465633</v>
+        <v>2014.8290932730913</v>
       </c>
       <c r="D1202" s="4"/>
       <c r="E1202" s="3"/>
@@ -16877,7 +16878,7 @@
         <v>95</v>
       </c>
       <c r="C1203">
-        <v>4599.9909273037474</v>
+        <v>135.46795443993946</v>
       </c>
       <c r="D1203" s="4"/>
       <c r="E1203" s="3"/>
@@ -16890,7 +16891,7 @@
         <v>96</v>
       </c>
       <c r="C1204">
-        <v>5662.3772985524438</v>
+        <v>596.84497484809549</v>
       </c>
       <c r="D1204" s="4"/>
       <c r="E1204" s="3"/>
@@ -16903,7 +16904,7 @@
         <v>97</v>
       </c>
       <c r="C1205">
-        <v>4637.3799069943188</v>
+        <v>1018.7434263612967</v>
       </c>
       <c r="D1205" s="4"/>
       <c r="E1205" s="3"/>
@@ -16916,7 +16917,7 @@
         <v>146</v>
       </c>
       <c r="C1206">
-        <v>6136.0396142478794</v>
+        <v>1045.9108656135813</v>
       </c>
       <c r="D1206" s="4"/>
       <c r="E1206" s="3"/>
@@ -16929,7 +16930,7 @@
         <v>10</v>
       </c>
       <c r="C1207">
-        <v>6575.9076682656223</v>
+        <v>790.05356262485509</v>
       </c>
       <c r="D1207" s="4"/>
       <c r="E1207" s="3"/>
@@ -16942,7 +16943,7 @@
         <v>147</v>
       </c>
       <c r="C1208">
-        <v>6311.280226019463</v>
+        <v>1447.7555388518574</v>
       </c>
       <c r="D1208" s="4"/>
       <c r="E1208" s="3"/>
@@ -16955,7 +16956,7 @@
         <v>99</v>
       </c>
       <c r="C1209">
-        <v>5036.4820033893475</v>
+        <v>705.88204376623082</v>
       </c>
       <c r="D1209" s="4"/>
       <c r="E1209" s="3"/>
@@ -16968,7 +16969,7 @@
         <v>62</v>
       </c>
       <c r="C1210">
-        <v>5446.617376125686</v>
+        <v>405.57500798206081</v>
       </c>
       <c r="D1210" s="4"/>
       <c r="E1210" s="3"/>
@@ -16981,7 +16982,7 @@
         <v>100</v>
       </c>
       <c r="C1211">
-        <v>6680.3740130159676</v>
+        <v>1023.9100133325994</v>
       </c>
       <c r="D1211" s="4"/>
       <c r="E1211" s="3"/>
@@ -16994,7 +16995,7 @@
         <v>148</v>
       </c>
       <c r="C1212">
-        <v>6040.1935917389956</v>
+        <v>504.78800229314169</v>
       </c>
       <c r="D1212" s="4"/>
       <c r="E1212" s="3"/>
@@ -17007,7 +17008,7 @@
         <v>149</v>
       </c>
       <c r="C1213">
-        <v>4568.2205629832733</v>
+        <v>1224.0763048117467</v>
       </c>
       <c r="D1213" s="4"/>
       <c r="E1213" s="3"/>
@@ -17020,7 +17021,7 @@
         <v>150</v>
       </c>
       <c r="C1214">
-        <v>4488.4506029441327</v>
+        <v>1289.7754257183374</v>
       </c>
       <c r="D1214" s="4"/>
       <c r="E1214" s="3"/>
@@ -17033,7 +17034,7 @@
         <v>101</v>
       </c>
       <c r="C1215">
-        <v>5573.1207357789108</v>
+        <v>1278.8674583593668</v>
       </c>
       <c r="D1215" s="4"/>
       <c r="E1215" s="3"/>
@@ -17046,7 +17047,7 @@
         <v>151</v>
       </c>
       <c r="C1216">
-        <v>5111.8821078422634</v>
+        <v>2142.498444707509</v>
       </c>
       <c r="D1216" s="4"/>
       <c r="E1216" s="3"/>
@@ -17059,7 +17060,7 @@
         <v>102</v>
       </c>
       <c r="C1217">
-        <v>4872.1583914264147</v>
+        <v>1954.3799402831571</v>
       </c>
       <c r="D1217" s="4"/>
       <c r="E1217" s="3"/>
@@ -17072,7 +17073,7 @@
         <v>103</v>
       </c>
       <c r="C1218">
-        <v>6501.6312541117823</v>
+        <v>1478.2809463969149</v>
       </c>
       <c r="D1218" s="4"/>
       <c r="E1218" s="3"/>
@@ -17085,7 +17086,7 @@
         <v>152</v>
       </c>
       <c r="C1219">
-        <v>5345.9382092925853</v>
+        <v>866.95758050947791</v>
       </c>
       <c r="D1219" s="4"/>
       <c r="E1219" s="3"/>
@@ -17098,7 +17099,7 @@
         <v>104</v>
       </c>
       <c r="C1220">
-        <v>5166.1710757430337</v>
+        <v>627.89861572940083</v>
       </c>
       <c r="D1220" s="4"/>
       <c r="E1220" s="3"/>
@@ -17111,7 +17112,7 @@
         <v>105</v>
       </c>
       <c r="C1221">
-        <v>5112.7526170589963</v>
+        <v>1415.2183942667461</v>
       </c>
       <c r="D1221" s="4"/>
       <c r="E1221" s="3"/>
@@ -17124,7 +17125,7 @@
         <v>106</v>
       </c>
       <c r="C1222">
-        <v>5177.1411152769524</v>
+        <v>2174.9749799088559</v>
       </c>
       <c r="D1222" s="4"/>
       <c r="E1222" s="3"/>
@@ -17137,7 +17138,7 @@
         <v>107</v>
       </c>
       <c r="C1223">
-        <v>5265.9847840512184</v>
+        <v>1134.1665362827782</v>
       </c>
       <c r="D1223" s="4"/>
       <c r="E1223" s="3"/>
@@ -17150,7 +17151,7 @@
         <v>108</v>
       </c>
       <c r="C1224">
-        <v>4688.2540565991521</v>
+        <v>2296.0020079908531</v>
       </c>
       <c r="D1224" s="4"/>
       <c r="E1224" s="3"/>
@@ -17163,7 +17164,7 @@
         <v>153</v>
       </c>
       <c r="C1225">
-        <v>5214.5562197591971</v>
+        <v>1356.7362663434706</v>
       </c>
       <c r="D1225" s="4"/>
       <c r="E1225" s="3"/>
@@ -17176,7 +17177,7 @@
         <v>109</v>
       </c>
       <c r="C1226">
-        <v>5146.5507001885217</v>
+        <v>1225.1256713806756</v>
       </c>
       <c r="D1226" s="4"/>
       <c r="E1226" s="3"/>
@@ -17189,7 +17190,7 @@
         <v>154</v>
       </c>
       <c r="C1227">
-        <v>6310.3344011857707</v>
+        <v>713.55675200824544</v>
       </c>
       <c r="D1227" s="4"/>
       <c r="E1227" s="3"/>
@@ -17202,7 +17203,7 @@
         <v>155</v>
       </c>
       <c r="C1228">
-        <v>6263.1247635078425</v>
+        <v>1310.4614569450259</v>
       </c>
       <c r="D1228" s="4"/>
       <c r="E1228" s="3"/>
@@ -17215,7 +17216,7 @@
         <v>110</v>
       </c>
       <c r="C1229">
-        <v>7522.9602368338856</v>
+        <v>2393.4323359011828</v>
       </c>
       <c r="D1229" s="4"/>
       <c r="E1229" s="3"/>
@@ -17228,7 +17229,7 @@
         <v>111</v>
       </c>
       <c r="C1230">
-        <v>5176.8862479082181</v>
+        <v>1371.6035768538638</v>
       </c>
       <c r="D1230" s="4"/>
       <c r="E1230" s="3"/>
@@ -17241,7 +17242,7 @@
         <v>112</v>
       </c>
       <c r="C1231">
-        <v>5179.3236429706203</v>
+        <v>1968.716679648941</v>
       </c>
       <c r="D1231" s="4"/>
       <c r="E1231" s="3"/>
@@ -17254,7 +17255,7 @@
         <v>156</v>
       </c>
       <c r="C1232">
-        <v>4908.5638435814662</v>
+        <v>1003.64522803816</v>
       </c>
       <c r="D1232" s="4"/>
       <c r="E1232" s="3"/>
@@ -17267,7 +17268,7 @@
         <v>157</v>
       </c>
       <c r="C1233">
-        <v>5008.627974499148</v>
+        <v>1003.64522803816</v>
       </c>
       <c r="D1233" s="4"/>
       <c r="E1233" s="3"/>
@@ -17280,7 +17281,7 @@
         <v>61</v>
       </c>
       <c r="C1234">
-        <v>5948.6489182792611</v>
+        <v>2302.4661737584074</v>
       </c>
       <c r="D1234" s="4"/>
       <c r="E1234" s="3"/>
@@ -17293,7 +17294,7 @@
         <v>158</v>
       </c>
       <c r="C1235">
-        <v>6112.7017734703495</v>
+        <v>1564.4408798679469</v>
       </c>
       <c r="D1235" s="4"/>
       <c r="E1235" s="3"/>
@@ -17306,7 +17307,7 @@
         <v>113</v>
       </c>
       <c r="C1236">
-        <v>5838.1087066929776</v>
+        <v>1135.62039195597</v>
       </c>
       <c r="D1236" s="4"/>
       <c r="E1236" s="3"/>
@@ -17319,7 +17320,7 @@
         <v>114</v>
       </c>
       <c r="C1237">
-        <v>4566.3115991109134</v>
+        <v>1926.2145089820269</v>
       </c>
       <c r="D1237" s="4"/>
       <c r="E1237" s="3"/>
@@ -17332,7 +17333,7 @@
         <v>115</v>
       </c>
       <c r="C1238">
-        <v>5253.1007136568969</v>
+        <v>1473.5387611674037</v>
       </c>
       <c r="D1238" s="4"/>
       <c r="E1238" s="3"/>
@@ -17345,7 +17346,7 @@
         <v>159</v>
       </c>
       <c r="C1239">
-        <v>5150.4734850160776</v>
+        <v>803.92232194030464</v>
       </c>
       <c r="D1239" s="4"/>
       <c r="E1239" s="3"/>
@@ -17358,7 +17359,7 @@
         <v>116</v>
       </c>
       <c r="C1240">
-        <v>4718.8604461153764</v>
+        <v>1301.4528605007804</v>
       </c>
       <c r="D1240" s="4"/>
       <c r="E1240" s="3"/>
@@ -17371,7 +17372,7 @@
         <v>117</v>
       </c>
       <c r="C1241">
-        <v>6398.1223012209875</v>
+        <v>946.08749489208265</v>
       </c>
       <c r="D1241" s="4"/>
       <c r="E1241" s="3"/>
@@ -17384,7 +17385,7 @@
         <v>98</v>
       </c>
       <c r="C1242">
-        <v>5811.4891472932995</v>
+        <v>1253.5116993969236</v>
       </c>
       <c r="D1242" s="4"/>
       <c r="E1242" s="3"/>
@@ -17397,7 +17398,7 @@
         <v>17</v>
       </c>
       <c r="C1243">
-        <v>8641.7529488894033</v>
+        <v>1174.9464865190289</v>
       </c>
       <c r="D1243" s="4"/>
       <c r="E1243" s="3"/>
@@ -17410,7 +17411,7 @@
         <v>18</v>
       </c>
       <c r="C1244">
-        <v>8253.0771909493542</v>
+        <v>1470.313015276527</v>
       </c>
       <c r="D1244" s="4"/>
       <c r="E1244" s="3"/>
@@ -17423,7 +17424,7 @@
         <v>19</v>
       </c>
       <c r="C1245">
-        <v>7898.3453895488647</v>
+        <v>2293.8132426088523</v>
       </c>
       <c r="D1245" s="4"/>
       <c r="E1245" s="3"/>
@@ -17436,7 +17437,7 @@
         <v>118</v>
       </c>
       <c r="C1246">
-        <v>7949.6472287362476</v>
+        <v>1317.5905868023258</v>
       </c>
       <c r="D1246" s="4"/>
       <c r="E1246" s="3"/>
@@ -17449,7 +17450,7 @@
         <v>3</v>
       </c>
       <c r="C1247">
-        <v>8821.6490881224745</v>
+        <v>1317.5808599900579</v>
       </c>
       <c r="D1247" s="4"/>
       <c r="E1247" s="3"/>
@@ -17462,7 +17463,7 @@
         <v>119</v>
       </c>
       <c r="C1248">
-        <v>8800.1895324061461</v>
+        <v>1363.2821751350198</v>
       </c>
       <c r="D1248" s="4"/>
       <c r="E1248" s="3"/>
@@ -17475,7 +17476,7 @@
         <v>21</v>
       </c>
       <c r="C1249">
-        <v>8570.3739804122488</v>
+        <v>1321.406744238174</v>
       </c>
       <c r="D1249" s="4"/>
       <c r="E1249" s="3"/>
@@ -17488,7 +17489,7 @@
         <v>22</v>
       </c>
       <c r="C1250">
-        <v>8961.5786339017632</v>
+        <v>1232.8383747286027</v>
       </c>
       <c r="D1250" s="4"/>
       <c r="E1250" s="3"/>
@@ -17501,7 +17502,7 @@
         <v>120</v>
       </c>
       <c r="C1251">
-        <v>8969.1569275191705</v>
+        <v>953.85364522354666</v>
       </c>
       <c r="D1251" s="4"/>
       <c r="E1251" s="3"/>
@@ -17514,7 +17515,7 @@
         <v>6</v>
       </c>
       <c r="C1252">
-        <v>9156.8715768125621</v>
+        <v>947.27172418540295</v>
       </c>
       <c r="D1252" s="4"/>
       <c r="E1252" s="3"/>
@@ -17527,7 +17528,7 @@
         <v>23</v>
       </c>
       <c r="C1253">
-        <v>8904.1296789347234</v>
+        <v>515.30893151076964</v>
       </c>
       <c r="D1253" s="4"/>
       <c r="E1253" s="3"/>
@@ -17540,7 +17541,7 @@
         <v>121</v>
       </c>
       <c r="C1254">
-        <v>8831.4104135005637</v>
+        <v>412.53735645687436</v>
       </c>
       <c r="D1254" s="4"/>
       <c r="E1254" s="3"/>
@@ -17553,7 +17554,7 @@
         <v>24</v>
       </c>
       <c r="C1255">
-        <v>8818.8223235341029</v>
+        <v>974.56020845106741</v>
       </c>
       <c r="D1255" s="4"/>
       <c r="E1255" s="3"/>
@@ -17566,7 +17567,7 @@
         <v>122</v>
       </c>
       <c r="C1256">
-        <v>7806.8476788713688</v>
+        <v>2105.5760778884774</v>
       </c>
       <c r="D1256" s="4"/>
       <c r="E1256" s="3"/>
@@ -17579,7 +17580,7 @@
         <v>26</v>
       </c>
       <c r="C1257">
-        <v>7753.5527676112033</v>
+        <v>2545.0297647943453</v>
       </c>
       <c r="D1257" s="4"/>
       <c r="E1257" s="3"/>
@@ -17592,7 +17593,7 @@
         <v>27</v>
       </c>
       <c r="C1258">
-        <v>8356.7402319434914</v>
+        <v>2545.0297647943453</v>
       </c>
       <c r="D1258" s="4"/>
       <c r="E1258" s="3"/>
@@ -17605,7 +17606,7 @@
         <v>28</v>
       </c>
       <c r="C1259">
-        <v>8897.8326177800463</v>
+        <v>1207.8376215143089</v>
       </c>
       <c r="D1259" s="4"/>
       <c r="E1259" s="3"/>
@@ -17618,7 +17619,7 @@
         <v>29</v>
       </c>
       <c r="C1260">
-        <v>7863.480901110428</v>
+        <v>1068.2232722629981</v>
       </c>
       <c r="D1260" s="4"/>
       <c r="E1260" s="3"/>
@@ -17631,7 +17632,7 @@
         <v>123</v>
       </c>
       <c r="C1261">
-        <v>8574.4856799341396</v>
+        <v>156.28753828999487</v>
       </c>
       <c r="D1261" s="4"/>
       <c r="E1261" s="3"/>
@@ -17644,7 +17645,7 @@
         <v>124</v>
       </c>
       <c r="C1262">
-        <v>8385.1975792497797</v>
+        <v>2336.2655606391186</v>
       </c>
       <c r="D1262" s="4"/>
       <c r="E1262" s="3"/>
@@ -17657,7 +17658,7 @@
         <v>30</v>
       </c>
       <c r="C1263">
-        <v>8846.8098131276165</v>
+        <v>285.60133004581149</v>
       </c>
       <c r="D1263" s="4"/>
       <c r="E1263" s="3"/>
@@ -17670,7 +17671,7 @@
         <v>31</v>
       </c>
       <c r="C1264">
-        <v>8382.7581286603472</v>
+        <v>344.75155680759241</v>
       </c>
       <c r="D1264" s="4"/>
       <c r="E1264" s="3"/>
@@ -17683,7 +17684,7 @@
         <v>32</v>
       </c>
       <c r="C1265">
-        <v>8482.5870246049617</v>
+        <v>347.22454885123136</v>
       </c>
       <c r="D1265" s="4"/>
       <c r="E1265" s="3"/>
@@ -17696,7 +17697,7 @@
         <v>33</v>
       </c>
       <c r="C1266">
-        <v>8825.2403472873848</v>
+        <v>2105.2629427771303</v>
       </c>
       <c r="D1266" s="4"/>
       <c r="E1266" s="3"/>
@@ -17709,7 +17710,7 @@
         <v>34</v>
       </c>
       <c r="C1267">
-        <v>9152.5012296389141</v>
+        <v>2182.2670122620048</v>
       </c>
       <c r="D1267" s="4"/>
       <c r="E1267" s="3"/>
@@ -17722,7 +17723,7 @@
         <v>35</v>
       </c>
       <c r="C1268">
-        <v>8575.6258077054445</v>
+        <v>1167.3388752376686</v>
       </c>
       <c r="D1268" s="4"/>
       <c r="E1268" s="3"/>
@@ -17735,7 +17736,7 @@
         <v>36</v>
       </c>
       <c r="C1269">
-        <v>8571.2958840213432</v>
+        <v>1179.8956993984216</v>
       </c>
       <c r="D1269" s="4"/>
       <c r="E1269" s="3"/>
@@ -17748,7 +17749,7 @@
         <v>37</v>
       </c>
       <c r="C1270">
-        <v>8987.3156730773808</v>
+        <v>215.84564193065026</v>
       </c>
       <c r="D1270" s="4"/>
       <c r="E1270" s="3"/>
@@ -17761,7 +17762,7 @@
         <v>38</v>
       </c>
       <c r="C1271">
-        <v>8633.0284625630393</v>
+        <v>304.89169749011228</v>
       </c>
       <c r="D1271" s="4"/>
       <c r="E1271" s="3"/>
@@ -17774,7 +17775,7 @@
         <v>39</v>
       </c>
       <c r="C1272">
-        <v>8949.1452456089901</v>
+        <v>1853.5946906118575</v>
       </c>
       <c r="D1272" s="4"/>
       <c r="E1272" s="3"/>
@@ -17787,7 +17788,7 @@
         <v>40</v>
       </c>
       <c r="C1273">
-        <v>9189.0677545955787</v>
+        <v>1107.0145533752966</v>
       </c>
       <c r="D1273" s="4"/>
       <c r="E1273" s="3"/>
@@ -17800,7 +17801,7 @@
         <v>41</v>
       </c>
       <c r="C1274">
-        <v>9049.0075649434275</v>
+        <v>598.09299282034578</v>
       </c>
       <c r="D1274" s="4"/>
       <c r="E1274" s="3"/>
@@ -17813,7 +17814,7 @@
         <v>9</v>
       </c>
       <c r="C1275">
-        <v>9214.0839672300826</v>
+        <v>1486.7970100057564</v>
       </c>
       <c r="D1275" s="4"/>
       <c r="E1275" s="3"/>
@@ -17826,7 +17827,7 @@
         <v>42</v>
       </c>
       <c r="C1276">
-        <v>8991.189582376177</v>
+        <v>484.81759303154917</v>
       </c>
       <c r="D1276" s="4"/>
       <c r="E1276" s="3"/>
@@ -17839,7 +17840,7 @@
         <v>125</v>
       </c>
       <c r="C1277">
-        <v>8372.310120894108</v>
+        <v>586.99316450338233</v>
       </c>
       <c r="D1277" s="4"/>
       <c r="E1277" s="3"/>
@@ -17852,7 +17853,7 @@
         <v>43</v>
       </c>
       <c r="C1278">
-        <v>7803.7519674573441</v>
+        <v>280.70459886741105</v>
       </c>
       <c r="D1278" s="4"/>
       <c r="E1278" s="3"/>
@@ -17865,7 +17866,7 @@
         <v>44</v>
       </c>
       <c r="C1279">
-        <v>7865.0209651431078</v>
+        <v>1927.5622019110172</v>
       </c>
       <c r="D1279" s="4"/>
       <c r="E1279" s="3"/>
@@ -17878,7 +17879,7 @@
         <v>45</v>
       </c>
       <c r="C1280">
-        <v>9011.5453119229896</v>
+        <v>1008.8403020769318</v>
       </c>
       <c r="D1280" s="4"/>
       <c r="E1280" s="3"/>
@@ -17891,7 +17892,7 @@
         <v>126</v>
       </c>
       <c r="C1281">
-        <v>9493.0612347664974</v>
+        <v>1032.6745541362309</v>
       </c>
       <c r="D1281" s="4"/>
       <c r="E1281" s="3"/>
@@ -17904,7 +17905,7 @@
         <v>127</v>
       </c>
       <c r="C1282">
-        <v>9311.0715651324281</v>
+        <v>1870.6435833146011</v>
       </c>
       <c r="D1282" s="4"/>
       <c r="E1282" s="3"/>
@@ -17917,7 +17918,7 @@
         <v>46</v>
       </c>
       <c r="C1283">
-        <v>8665.9525065957132</v>
+        <v>1469.6059134252764</v>
       </c>
       <c r="D1283" s="4"/>
       <c r="E1283" s="3"/>
@@ -17930,7 +17931,7 @@
         <v>47</v>
       </c>
       <c r="C1284">
-        <v>8606.7270946927947</v>
+        <v>1572.2543293527142</v>
       </c>
       <c r="D1284" s="4"/>
       <c r="E1284" s="3"/>
@@ -17943,7 +17944,7 @@
         <v>48</v>
       </c>
       <c r="C1285">
-        <v>9204.6913876437175</v>
+        <v>1395.0664619402805</v>
       </c>
       <c r="D1285" s="4"/>
       <c r="E1285" s="3"/>
@@ -17956,7 +17957,7 @@
         <v>128</v>
       </c>
       <c r="C1286">
-        <v>8905.4607241462872</v>
+        <v>1054.4092091939058</v>
       </c>
       <c r="D1286" s="4"/>
       <c r="E1286" s="3"/>
@@ -17969,7 +17970,7 @@
         <v>49</v>
       </c>
       <c r="C1287">
-        <v>8746.8816969056024</v>
+        <v>1524.9805467193391</v>
       </c>
       <c r="D1287" s="4"/>
       <c r="E1287" s="3"/>
@@ -17982,7 +17983,7 @@
         <v>50</v>
       </c>
       <c r="C1288">
-        <v>8587.8028669709147</v>
+        <v>2938.659208955653</v>
       </c>
       <c r="D1288" s="4"/>
       <c r="E1288" s="3"/>
@@ -17995,7 +17996,7 @@
         <v>51</v>
       </c>
       <c r="C1289">
-        <v>9351.1607689956272</v>
+        <v>292.47144182850155</v>
       </c>
       <c r="D1289" s="4"/>
       <c r="E1289" s="3"/>
@@ -18008,7 +18009,7 @@
         <v>52</v>
       </c>
       <c r="C1290">
-        <v>8981.4732519373629</v>
+        <v>209.18763387548762</v>
       </c>
       <c r="D1290" s="4"/>
       <c r="E1290" s="3"/>
@@ -18021,7 +18022,7 @@
         <v>16</v>
       </c>
       <c r="C1291">
-        <v>8475.4084435868062</v>
+        <v>2059.8131049316244</v>
       </c>
       <c r="D1291" s="4"/>
       <c r="E1291" s="3"/>
@@ -18034,7 +18035,7 @@
         <v>53</v>
       </c>
       <c r="C1292">
-        <v>8048.1658904897922</v>
+        <v>1248.0417549188953</v>
       </c>
       <c r="D1292" s="4"/>
       <c r="E1292" s="3"/>
@@ -18047,7 +18048,7 @@
         <v>54</v>
       </c>
       <c r="C1293">
-        <v>9223.4249652393228</v>
+        <v>1428.2518342309445</v>
       </c>
       <c r="D1293" s="4"/>
       <c r="E1293" s="3"/>
@@ -18060,7 +18061,7 @@
         <v>55</v>
       </c>
       <c r="C1294">
-        <v>8417.020258768307</v>
+        <v>1341.1851866989653</v>
       </c>
       <c r="D1294" s="4"/>
       <c r="E1294" s="3"/>
@@ -18073,7 +18074,7 @@
         <v>56</v>
       </c>
       <c r="C1295">
-        <v>8789.3583812069992</v>
+        <v>1183.7699688281634</v>
       </c>
       <c r="D1295" s="4"/>
       <c r="E1295" s="3"/>
@@ -18086,7 +18087,7 @@
         <v>57</v>
       </c>
       <c r="C1296">
-        <v>9328.0801440050491</v>
+        <v>1998.078121485853</v>
       </c>
       <c r="D1296" s="4"/>
       <c r="E1296" s="3"/>
@@ -18099,7 +18100,7 @@
         <v>58</v>
       </c>
       <c r="C1297">
-        <v>8721.8220359580919</v>
+        <v>2302.473144402235</v>
       </c>
       <c r="D1297" s="4"/>
       <c r="E1297" s="3"/>
@@ -18112,7 +18113,7 @@
         <v>59</v>
       </c>
       <c r="C1298">
-        <v>9137.2037691189653</v>
+        <v>2330.3249121171975</v>
       </c>
       <c r="D1298" s="4"/>
       <c r="E1298" s="3"/>
@@ -18125,7 +18126,7 @@
         <v>15</v>
       </c>
       <c r="C1299">
-        <v>8665.7031138210205</v>
+        <v>1760.5549989115393</v>
       </c>
       <c r="D1299" s="4"/>
       <c r="E1299" s="3"/>
@@ -18138,7 +18139,7 @@
         <v>129</v>
       </c>
       <c r="C1300">
-        <v>7738.9784874579163</v>
+        <v>927.22235775161255</v>
       </c>
       <c r="D1300" s="4"/>
       <c r="E1300" s="3"/>
@@ -18151,7 +18152,7 @@
         <v>60</v>
       </c>
       <c r="C1301">
-        <v>8594.2303904526361</v>
+        <v>915.17767047856034</v>
       </c>
       <c r="D1301" s="4"/>
       <c r="E1301" s="3"/>
@@ -18164,7 +18165,7 @@
         <v>130</v>
       </c>
       <c r="C1302">
-        <v>8387.0822791388091</v>
+        <v>1222.0117078496269</v>
       </c>
       <c r="D1302" s="4"/>
       <c r="E1302" s="3"/>
@@ -18177,7 +18178,7 @@
         <v>62</v>
       </c>
       <c r="C1303">
-        <v>9138.5909507936412</v>
+        <v>298.48669969500196</v>
       </c>
       <c r="D1303" s="4"/>
       <c r="E1303" s="3"/>
@@ -18190,7 +18191,7 @@
         <v>7</v>
       </c>
       <c r="C1304">
-        <v>9461.8075694282106</v>
+        <v>963.44514363895848</v>
       </c>
       <c r="D1304" s="4"/>
       <c r="E1304" s="3"/>
@@ -18203,7 +18204,7 @@
         <v>131</v>
       </c>
       <c r="C1305">
-        <v>8525.6039537572578</v>
+        <v>1041.6902701512695</v>
       </c>
       <c r="D1305" s="4"/>
       <c r="E1305" s="3"/>
@@ -18216,7 +18217,7 @@
         <v>63</v>
       </c>
       <c r="C1306">
-        <v>8328.1544863988529</v>
+        <v>2050.4112459753819</v>
       </c>
       <c r="D1306" s="4"/>
       <c r="E1306" s="3"/>
@@ -18229,7 +18230,7 @@
         <v>64</v>
       </c>
       <c r="C1307">
-        <v>9190.2337028011589</v>
+        <v>1344.2695249123606</v>
       </c>
       <c r="D1307" s="4"/>
       <c r="E1307" s="3"/>
@@ -18242,7 +18243,7 @@
         <v>65</v>
       </c>
       <c r="C1308">
-        <v>8944.7866007925695</v>
+        <v>2154.3003807527753</v>
       </c>
       <c r="D1308" s="4"/>
       <c r="E1308" s="3"/>
@@ -18255,7 +18256,7 @@
         <v>12</v>
       </c>
       <c r="C1309">
-        <v>8603.328486446766</v>
+        <v>1239.5599017661252</v>
       </c>
       <c r="D1309" s="4"/>
       <c r="E1309" s="3"/>
@@ -18268,7 +18269,7 @@
         <v>66</v>
       </c>
       <c r="C1310">
-        <v>9224.1399688839283</v>
+        <v>575.768935630545</v>
       </c>
       <c r="D1310" s="4"/>
       <c r="E1310" s="3"/>
@@ -18281,7 +18282,7 @@
         <v>67</v>
       </c>
       <c r="C1311">
-        <v>8333.2581854433083</v>
+        <v>1361.8726654424613</v>
       </c>
       <c r="D1311" s="4"/>
       <c r="E1311" s="3"/>
@@ -18294,7 +18295,7 @@
         <v>132</v>
       </c>
       <c r="C1312">
-        <v>9150.4954193384492</v>
+        <v>1254.1273734781682</v>
       </c>
       <c r="D1312" s="4"/>
       <c r="E1312" s="3"/>
@@ -18307,7 +18308,7 @@
         <v>68</v>
       </c>
       <c r="C1313">
-        <v>8147.5670021983851</v>
+        <v>1093.5532481857006</v>
       </c>
       <c r="D1313" s="4"/>
       <c r="E1313" s="3"/>
@@ -18320,7 +18321,7 @@
         <v>69</v>
       </c>
       <c r="C1314">
-        <v>8629.9127434228321</v>
+        <v>2048.4599049783492</v>
       </c>
       <c r="D1314" s="4"/>
       <c r="E1314" s="3"/>
@@ -18333,7 +18334,7 @@
         <v>70</v>
       </c>
       <c r="C1315">
-        <v>9287.6691959450163</v>
+        <v>981.14698568207984</v>
       </c>
       <c r="D1315" s="4"/>
       <c r="E1315" s="3"/>
@@ -18346,7 +18347,7 @@
         <v>71</v>
       </c>
       <c r="C1316">
-        <v>8994.9867681398046</v>
+        <v>1547.3223392493912</v>
       </c>
       <c r="D1316" s="4"/>
       <c r="E1316" s="3"/>
@@ -18359,7 +18360,7 @@
         <v>1</v>
       </c>
       <c r="C1317">
-        <v>8801.3891911196388</v>
+        <v>971.93242725122309</v>
       </c>
       <c r="D1317" s="4"/>
       <c r="E1317" s="3"/>
@@ -18372,7 +18373,7 @@
         <v>72</v>
       </c>
       <c r="C1318">
-        <v>8553.4036439033462</v>
+        <v>1749.9082257192831</v>
       </c>
       <c r="D1318" s="4"/>
       <c r="E1318" s="3"/>
@@ -18385,7 +18386,7 @@
         <v>73</v>
       </c>
       <c r="C1319">
-        <v>8687.6799021393344</v>
+        <v>2863.5614533712483</v>
       </c>
       <c r="D1319" s="4"/>
       <c r="E1319" s="3"/>
@@ -18398,7 +18399,7 @@
         <v>133</v>
       </c>
       <c r="C1320">
-        <v>9376.7156627274489</v>
+        <v>1009.6702243737061</v>
       </c>
       <c r="D1320" s="4"/>
       <c r="E1320" s="3"/>
@@ -18411,7 +18412,7 @@
         <v>74</v>
       </c>
       <c r="C1321">
-        <v>8472.9218388714307</v>
+        <v>619.95030365661989</v>
       </c>
       <c r="D1321" s="4"/>
       <c r="E1321" s="3"/>
@@ -18424,7 +18425,7 @@
         <v>75</v>
       </c>
       <c r="C1322">
-        <v>7983.6543154979263</v>
+        <v>1369.3845891404319</v>
       </c>
       <c r="D1322" s="4"/>
       <c r="E1322" s="3"/>
@@ -18437,7 +18438,7 @@
         <v>76</v>
       </c>
       <c r="C1323">
-        <v>8622.3059845301686</v>
+        <v>1212.6915393785719</v>
       </c>
       <c r="D1323" s="4"/>
       <c r="E1323" s="3"/>
@@ -18450,7 +18451,7 @@
         <v>134</v>
       </c>
       <c r="C1324">
-        <v>8888.339231241087</v>
+        <v>1217.003997310964</v>
       </c>
       <c r="D1324" s="4"/>
       <c r="E1324" s="3"/>
@@ -18463,7 +18464,7 @@
         <v>77</v>
       </c>
       <c r="C1325">
-        <v>8376.8448982253612</v>
+        <v>2263.4471834445967</v>
       </c>
       <c r="D1325" s="4"/>
       <c r="E1325" s="3"/>
@@ -18476,7 +18477,7 @@
         <v>78</v>
       </c>
       <c r="C1326">
-        <v>8106.3606696152947</v>
+        <v>839.11344434501734</v>
       </c>
       <c r="D1326" s="4"/>
       <c r="E1326" s="3"/>
@@ -18489,7 +18490,7 @@
         <v>79</v>
       </c>
       <c r="C1327">
-        <v>8960.9946189006769</v>
+        <v>2118.6747233441179</v>
       </c>
       <c r="D1327" s="4"/>
       <c r="E1327" s="3"/>
@@ -18502,7 +18503,7 @@
         <v>80</v>
       </c>
       <c r="C1328">
-        <v>8478.4837488359444</v>
+        <v>2184.888140992744</v>
       </c>
       <c r="D1328" s="4"/>
       <c r="E1328" s="3"/>
@@ -18515,7 +18516,7 @@
         <v>81</v>
       </c>
       <c r="C1329">
-        <v>8950.7277049772711</v>
+        <v>2109.6496610776308</v>
       </c>
       <c r="D1329" s="4"/>
       <c r="E1329" s="3"/>
@@ -18528,7 +18529,7 @@
         <v>82</v>
       </c>
       <c r="C1330">
-        <v>8941.1294196940253</v>
+        <v>1238.3679250447453</v>
       </c>
       <c r="D1330" s="4"/>
       <c r="E1330" s="3"/>
@@ -18541,7 +18542,7 @@
         <v>135</v>
       </c>
       <c r="C1331">
-        <v>9286.2563055912433</v>
+        <v>866.26929278068212</v>
       </c>
       <c r="D1331" s="4"/>
       <c r="E1331" s="3"/>
@@ -18554,7 +18555,7 @@
         <v>136</v>
       </c>
       <c r="C1332">
-        <v>8541.6523896068102</v>
+        <v>1766.7371373250671</v>
       </c>
       <c r="D1332" s="4"/>
       <c r="E1332" s="3"/>
@@ -18567,7 +18568,7 @@
         <v>83</v>
       </c>
       <c r="C1333">
-        <v>9140.9216684567127</v>
+        <v>956.84644459937078</v>
       </c>
       <c r="D1333" s="4"/>
       <c r="E1333" s="3"/>
@@ -18580,7 +18581,7 @@
         <v>137</v>
       </c>
       <c r="C1334">
-        <v>9241.3207862943182</v>
+        <v>455.09349089367885</v>
       </c>
       <c r="D1334" s="4"/>
       <c r="E1334" s="3"/>
@@ -18593,7 +18594,7 @@
         <v>84</v>
       </c>
       <c r="C1335">
-        <v>8938.8700307002327</v>
+        <v>474.95233536193717</v>
       </c>
       <c r="D1335" s="4"/>
       <c r="E1335" s="3"/>
@@ -18606,7 +18607,7 @@
         <v>85</v>
       </c>
       <c r="C1336">
-        <v>8706.3365978616548</v>
+        <v>1397.0213022334738</v>
       </c>
       <c r="D1336" s="4"/>
       <c r="E1336" s="3"/>
@@ -18619,7 +18620,7 @@
         <v>86</v>
       </c>
       <c r="C1337">
-        <v>8618.0217902979075</v>
+        <v>1028.7362493529251</v>
       </c>
       <c r="D1337" s="4"/>
       <c r="E1337" s="3"/>
@@ -18632,7 +18633,7 @@
         <v>87</v>
       </c>
       <c r="C1338">
-        <v>8628.2791866962907</v>
+        <v>264.44208336079964</v>
       </c>
       <c r="D1338" s="4"/>
       <c r="E1338" s="3"/>
@@ -18645,7 +18646,7 @@
         <v>88</v>
       </c>
       <c r="C1339">
-        <v>8651.8427628722511</v>
+        <v>817.49579556802007</v>
       </c>
       <c r="D1339" s="4"/>
       <c r="E1339" s="3"/>
@@ -18658,7 +18659,7 @@
         <v>89</v>
       </c>
       <c r="C1340">
-        <v>8722.6538098742567</v>
+        <v>35.350871576938822</v>
       </c>
       <c r="D1340" s="4"/>
       <c r="E1340" s="3"/>
@@ -18671,7 +18672,7 @@
         <v>138</v>
       </c>
       <c r="C1341">
-        <v>8928.8350447071061</v>
+        <v>923.83397869549538</v>
       </c>
       <c r="D1341" s="4"/>
       <c r="E1341" s="3"/>
@@ -18684,7 +18685,7 @@
         <v>90</v>
       </c>
       <c r="C1342">
-        <v>8647.5603629315683</v>
+        <v>971.23808903106431</v>
       </c>
       <c r="D1342" s="4"/>
       <c r="E1342" s="3"/>
@@ -18697,7 +18698,7 @@
         <v>25</v>
       </c>
       <c r="C1343">
-        <v>8337.7712320542596</v>
+        <v>2639.2359310549336</v>
       </c>
       <c r="D1343" s="4"/>
       <c r="E1343" s="3"/>
@@ -18710,7 +18711,7 @@
         <v>139</v>
       </c>
       <c r="C1344">
-        <v>8369.6593577946023</v>
+        <v>1623.8367249837413</v>
       </c>
       <c r="D1344" s="4"/>
       <c r="E1344" s="3"/>
@@ -18723,7 +18724,7 @@
         <v>140</v>
       </c>
       <c r="C1345">
-        <v>8855.6916578869532</v>
+        <v>1102.4219678900536</v>
       </c>
       <c r="D1345" s="4"/>
       <c r="E1345" s="3"/>
@@ -18736,7 +18737,7 @@
         <v>141</v>
       </c>
       <c r="C1346">
-        <v>9093.2167126733166</v>
+        <v>1052.3348230014467</v>
       </c>
       <c r="D1346" s="4"/>
       <c r="E1346" s="3"/>
@@ -18749,7 +18750,7 @@
         <v>91</v>
       </c>
       <c r="C1347">
-        <v>9230.0708450340499</v>
+        <v>1030.5290142356573</v>
       </c>
       <c r="D1347" s="4"/>
       <c r="E1347" s="3"/>
@@ -18762,7 +18763,7 @@
         <v>142</v>
       </c>
       <c r="C1348">
-        <v>9192.1491557626632</v>
+        <v>1493.7045094516334</v>
       </c>
       <c r="D1348" s="4"/>
       <c r="E1348" s="3"/>
@@ -18775,7 +18776,7 @@
         <v>92</v>
       </c>
       <c r="C1349">
-        <v>9341.8047063636441</v>
+        <v>2996.2964532665337</v>
       </c>
       <c r="D1349" s="4"/>
       <c r="E1349" s="3"/>
@@ -18788,7 +18789,7 @@
         <v>83</v>
       </c>
       <c r="C1350">
-        <v>9140.9216684567127</v>
+        <v>1395.34205597307</v>
       </c>
       <c r="D1350" s="4"/>
       <c r="E1350" s="3"/>
@@ -18801,7 +18802,7 @@
         <v>93</v>
       </c>
       <c r="C1351">
-        <v>8965.8607095451807</v>
+        <v>1202.9447616964105</v>
       </c>
       <c r="D1351" s="4"/>
       <c r="E1351" s="3"/>
@@ -18814,7 +18815,7 @@
         <v>143</v>
       </c>
       <c r="C1352">
-        <v>8960.381098217993</v>
+        <v>1234.0431692709394</v>
       </c>
       <c r="D1352" s="4"/>
       <c r="E1352" s="3"/>
@@ -18827,7 +18828,7 @@
         <v>94</v>
       </c>
       <c r="C1353">
-        <v>9114.7603470775703</v>
+        <v>1264.9767669970954</v>
       </c>
       <c r="D1353" s="4"/>
       <c r="E1353" s="3"/>
@@ -18840,7 +18841,7 @@
         <v>144</v>
       </c>
       <c r="C1354">
-        <v>9110.9070092223028</v>
+        <v>933.50639973249963</v>
       </c>
       <c r="D1354" s="4"/>
       <c r="E1354" s="3"/>
@@ -18853,7 +18854,7 @@
         <v>145</v>
       </c>
       <c r="C1355">
-        <v>9059.258461502588</v>
+        <v>569.42558102453677</v>
       </c>
       <c r="D1355" s="4"/>
       <c r="E1355" s="3"/>
@@ -18866,7 +18867,7 @@
         <v>95</v>
       </c>
       <c r="C1356">
-        <v>8303.0487718330587</v>
+        <v>2084.0398257513557</v>
       </c>
       <c r="D1356" s="4"/>
       <c r="E1356" s="3"/>
@@ -18879,7 +18880,7 @@
         <v>96</v>
       </c>
       <c r="C1357">
-        <v>8987.4310908914304</v>
+        <v>1579.3546584501448</v>
       </c>
       <c r="D1357" s="4"/>
       <c r="E1357" s="3"/>
@@ -18892,7 +18893,7 @@
         <v>97</v>
       </c>
       <c r="C1358">
-        <v>8531.8427106385989</v>
+        <v>1138.247388002954</v>
       </c>
       <c r="D1358" s="4"/>
       <c r="E1358" s="3"/>
@@ -18905,7 +18906,7 @@
         <v>146</v>
       </c>
       <c r="C1359">
-        <v>9017.6823221299346</v>
+        <v>1157.4919890295103</v>
       </c>
       <c r="D1359" s="4"/>
       <c r="E1359" s="3"/>
@@ -18918,7 +18919,7 @@
         <v>10</v>
       </c>
       <c r="C1360">
-        <v>9184.2599562563009</v>
+        <v>1459.4327165901248</v>
       </c>
       <c r="D1360" s="4"/>
       <c r="E1360" s="3"/>
@@ -18931,7 +18932,7 @@
         <v>147</v>
       </c>
       <c r="C1361">
-        <v>9521.9790547393386</v>
+        <v>764.78514725411105</v>
       </c>
       <c r="D1361" s="4"/>
       <c r="E1361" s="3"/>
@@ -18944,7 +18945,7 @@
         <v>99</v>
       </c>
       <c r="C1362">
-        <v>8819.4387535945898</v>
+        <v>2387.4431575200811</v>
       </c>
       <c r="D1362" s="4"/>
       <c r="E1362" s="3"/>
@@ -18957,7 +18958,7 @@
         <v>62</v>
       </c>
       <c r="C1363">
-        <v>9138.5909507936412</v>
+        <v>2402.5084181668199</v>
       </c>
       <c r="D1363" s="4"/>
       <c r="E1363" s="3"/>
@@ -18970,7 +18971,7 @@
         <v>100</v>
       </c>
       <c r="C1364">
-        <v>8822.4988209178555</v>
+        <v>1194.4218904066765</v>
       </c>
       <c r="D1364" s="4"/>
       <c r="E1364" s="3"/>
@@ -18983,7 +18984,7 @@
         <v>148</v>
       </c>
       <c r="C1365">
-        <v>8735.2125663673141</v>
+        <v>1680.3852911931253</v>
       </c>
       <c r="D1365" s="4"/>
       <c r="E1365" s="3"/>
@@ -18996,7 +18997,7 @@
         <v>149</v>
       </c>
       <c r="C1366">
-        <v>8535.2091078562607</v>
+        <v>954.8097825861214</v>
       </c>
       <c r="D1366" s="4"/>
       <c r="E1366" s="3"/>
@@ -19009,7 +19010,7 @@
         <v>150</v>
       </c>
       <c r="C1367">
-        <v>8507.7412284051788</v>
+        <v>865.86705914514152</v>
       </c>
       <c r="D1367" s="4"/>
       <c r="E1367" s="3"/>
@@ -19022,7 +19023,7 @@
         <v>101</v>
       </c>
       <c r="C1368">
-        <v>9068.3378031796547</v>
+        <v>892.90724373479713</v>
       </c>
       <c r="D1368" s="4"/>
       <c r="E1368" s="3"/>
@@ -19035,7 +19036,7 @@
         <v>151</v>
       </c>
       <c r="C1369">
-        <v>8902.132972225103</v>
+        <v>731.179540306435</v>
       </c>
       <c r="D1369" s="4"/>
       <c r="E1369" s="3"/>
@@ -19048,7 +19049,7 @@
         <v>102</v>
       </c>
       <c r="C1370">
-        <v>8858.6476307818903</v>
+        <v>547.2161075751103</v>
       </c>
       <c r="D1370" s="4"/>
       <c r="E1370" s="3"/>
@@ -19061,7 +19062,7 @@
         <v>103</v>
       </c>
       <c r="C1371">
-        <v>8894.8177154942568</v>
+        <v>862.70427779806312</v>
       </c>
       <c r="D1371" s="4"/>
       <c r="E1371" s="3"/>
@@ -19074,7 +19075,7 @@
         <v>152</v>
       </c>
       <c r="C1372">
-        <v>9252.1923120487445</v>
+        <v>1358.7567270351326</v>
       </c>
       <c r="D1372" s="4"/>
       <c r="E1372" s="3"/>
@@ -19087,7 +19088,7 @@
         <v>104</v>
       </c>
       <c r="C1373">
-        <v>8831.526144310923</v>
+        <v>1586.0985047720017</v>
       </c>
       <c r="D1373" s="4"/>
       <c r="E1373" s="3"/>
@@ -19100,7 +19101,7 @@
         <v>105</v>
       </c>
       <c r="C1374">
-        <v>9057.472736491738</v>
+        <v>819.30399117942386</v>
       </c>
       <c r="D1374" s="4"/>
       <c r="E1374" s="3"/>
@@ -19113,7 +19114,7 @@
         <v>106</v>
       </c>
       <c r="C1375">
-        <v>8962.8136282184187</v>
+        <v>67.552080560393165</v>
       </c>
       <c r="D1375" s="4"/>
       <c r="E1375" s="3"/>
@@ -19126,7 +19127,7 @@
         <v>107</v>
       </c>
       <c r="C1376">
-        <v>8867.6265578204911</v>
+        <v>2992.9574903849862</v>
       </c>
       <c r="D1376" s="4"/>
       <c r="E1376" s="3"/>
@@ -19139,7 +19140,7 @@
         <v>108</v>
       </c>
       <c r="C1377">
-        <v>8199.6297817542236</v>
+        <v>151.00150183346258</v>
       </c>
       <c r="D1377" s="4"/>
       <c r="E1377" s="3"/>
@@ -19152,7 +19153,7 @@
         <v>153</v>
       </c>
       <c r="C1378">
-        <v>8683.1102948392418</v>
+        <v>920.6854433915521</v>
       </c>
       <c r="D1378" s="4"/>
       <c r="E1378" s="3"/>
@@ -19165,7 +19166,7 @@
         <v>109</v>
       </c>
       <c r="C1379">
-        <v>8877.6999731956421</v>
+        <v>1066.6202706340696</v>
       </c>
       <c r="D1379" s="4"/>
       <c r="E1379" s="3"/>
@@ -19178,7 +19179,7 @@
         <v>154</v>
       </c>
       <c r="C1380">
-        <v>9522.5132855582542</v>
+        <v>1499.0232259765639</v>
       </c>
       <c r="D1380" s="4"/>
       <c r="E1380" s="3"/>
@@ -19191,7 +19192,7 @@
         <v>155</v>
       </c>
       <c r="C1381">
-        <v>8118.5529128760618</v>
+        <v>917.90383147863065</v>
       </c>
       <c r="D1381" s="4"/>
       <c r="E1381" s="3"/>
@@ -19204,7 +19205,7 @@
         <v>110</v>
       </c>
       <c r="C1382">
-        <v>9344.6475486161089</v>
+        <v>240.62778354213071</v>
       </c>
       <c r="D1382" s="4"/>
       <c r="E1382" s="3"/>
@@ -19217,7 +19218,7 @@
         <v>111</v>
       </c>
       <c r="C1383">
-        <v>8926.1688685575737</v>
+        <v>810.74441799893316</v>
       </c>
       <c r="D1383" s="4"/>
       <c r="E1383" s="3"/>
@@ -19230,7 +19231,7 @@
         <v>112</v>
       </c>
       <c r="C1384">
-        <v>8957.1171593126128</v>
+        <v>597.46462343621329</v>
       </c>
       <c r="D1384" s="4"/>
       <c r="E1384" s="3"/>
@@ -19243,7 +19244,7 @@
         <v>156</v>
       </c>
       <c r="C1385">
-        <v>9019.4463619452617</v>
+        <v>1309.3634367050624</v>
       </c>
       <c r="D1385" s="4"/>
       <c r="E1385" s="3"/>
@@ -19256,7 +19257,7 @@
         <v>157</v>
       </c>
       <c r="C1386">
-        <v>8895.9279366736009</v>
+        <v>1309.3634367050624</v>
       </c>
       <c r="D1386" s="4"/>
       <c r="E1386" s="3"/>
@@ -19269,7 +19270,7 @@
         <v>61</v>
       </c>
       <c r="C1387">
-        <v>8382.2472498646785</v>
+        <v>148.2089375014705</v>
       </c>
       <c r="D1387" s="4"/>
       <c r="E1387" s="3"/>
@@ -19282,7 +19283,7 @@
         <v>158</v>
       </c>
       <c r="C1388">
-        <v>8381.9524198022445</v>
+        <v>711.36156307193255</v>
       </c>
       <c r="D1388" s="4"/>
       <c r="E1388" s="3"/>
@@ -19295,7 +19296,7 @@
         <v>113</v>
       </c>
       <c r="C1389">
-        <v>8500.3305991475318</v>
+        <v>1028.7503036274152</v>
       </c>
       <c r="D1389" s="4"/>
       <c r="E1389" s="3"/>
@@ -19308,7 +19309,7 @@
         <v>114</v>
       </c>
       <c r="C1390">
-        <v>8476.737570101448</v>
+        <v>480.94839773188306</v>
       </c>
       <c r="D1390" s="4"/>
       <c r="E1390" s="3"/>
@@ -19321,7 +19322,7 @@
         <v>115</v>
       </c>
       <c r="C1391">
-        <v>8958.1775352512614</v>
+        <v>779.76973596402684</v>
       </c>
       <c r="D1391" s="4"/>
       <c r="E1391" s="3"/>
@@ -19334,7 +19335,7 @@
         <v>159</v>
       </c>
       <c r="C1392">
-        <v>8659.670469028857</v>
+        <v>1353.5144294398153</v>
       </c>
       <c r="D1392" s="4"/>
       <c r="E1392" s="3"/>
@@ -19347,7 +19348,7 @@
         <v>116</v>
       </c>
       <c r="C1393">
-        <v>8033.9410473122243</v>
+        <v>1037.4061459095942</v>
       </c>
       <c r="D1393" s="4"/>
       <c r="E1393" s="3"/>
@@ -19360,7 +19361,7 @@
         <v>117</v>
       </c>
       <c r="C1394">
-        <v>9227.3937717164954</v>
+        <v>1323.9776401966124</v>
       </c>
       <c r="D1394" s="4"/>
       <c r="E1394" s="3"/>
@@ -19373,7 +19374,7 @@
         <v>98</v>
       </c>
       <c r="C1395">
-        <v>8586.741272784142</v>
+        <v>996.8711456841786</v>
       </c>
       <c r="D1395" s="4"/>
       <c r="E1395" s="3"/>

</xml_diff>